<commit_message>
update data, extending implied inflation series
</commit_message>
<xml_diff>
--- a/Input/swaps/eur-inflation-HICPxT-swaps.xlsx
+++ b/Input/swaps/eur-inflation-HICPxT-swaps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\SHARE\cmf\Desi\Rajesh\POLICY\Inflation_Swap_Breakeven_Basis\input\swaps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\SHARE\cmf\Desi\Rajesh\IIE\Input\swaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D24A18-C21E-4732-ADA0-DA525EA141A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28B6FB4-79AD-42B6-8AD2-00F89F0067C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5865" yWindow="1200" windowWidth="19425" windowHeight="12045" xr2:uid="{43B30E9F-8D1A-4EAB-8504-0C8FB3A38EDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43B30E9F-8D1A-4EAB-8504-0C8FB3A38EDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,116 +191,116 @@
   <volType type="realTimeData">
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...4058645432</v>
+        <v>#N/A Requesting Data...1846912138</v>
         <stp/>
         <stp>BTODAY|10610048301435813905</stp>
+        <tr r="W3" s="1"/>
+        <tr r="O3" s="1"/>
+        <tr r="E3" s="1"/>
+        <tr r="G3" s="1"/>
         <tr r="AC3" s="1"/>
+        <tr r="Q3" s="1"/>
+        <tr r="I3" s="1"/>
+        <tr r="S3" s="1"/>
+        <tr r="K3" s="1"/>
+        <tr r="U3" s="1"/>
         <tr r="Y3" s="1"/>
-        <tr r="U3" s="1"/>
+        <tr r="M3" s="1"/>
+        <tr r="A3" s="1"/>
+        <tr r="C3" s="1"/>
         <tr r="AA3" s="1"/>
-        <tr r="G3" s="1"/>
-        <tr r="W3" s="1"/>
-        <tr r="E3" s="1"/>
-        <tr r="K3" s="1"/>
-        <tr r="C3" s="1"/>
-        <tr r="M3" s="1"/>
-        <tr r="Q3" s="1"/>
-        <tr r="S3" s="1"/>
-        <tr r="A3" s="1"/>
-        <tr r="I3" s="1"/>
-        <tr r="O3" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|14727609673807760966</stp>
-        <tr r="K3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|15653923395037529094</stp>
-        <tr r="S3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|12272595237080073447</stp>
-        <tr r="I3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|14441468188519197158</stp>
+        <stp>BDH|13635314096660805235</stp>
         <tr r="M3" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|15716841991645468746</stp>
+        <stp>BDH|12535776639532594737</stp>
+        <tr r="G3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|11931716834053685603</stp>
         <tr r="E3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|13066307407236801762</stp>
+        <tr r="AA3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|11091778390002020832</stp>
+        <tr r="O3" s="1"/>
       </tp>
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|9695688149684394347</stp>
+        <stp>BDH|7432321582823799209</stp>
+        <tr r="Y3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|7949973141835531017</stp>
+        <tr r="I3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|8216579873721617135</stp>
+        <tr r="AC3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|1972534724420298299</stp>
+        <tr r="W3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|2197307417585166338</stp>
         <tr r="A3" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|4305635298085579773</stp>
-        <tr r="AA3" s="1"/>
+        <stp>BDH|1791991040416734868</stp>
+        <tr r="U3" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|7329939505106391159</stp>
-        <tr r="Y3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|9580763817411231751</stp>
+        <stp>BDH|4582328516234055112</stp>
         <tr r="Q3" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|2093428132028452605</stp>
-        <tr r="G3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|1831583759547008234</stp>
-        <tr r="W3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|4871150062744190748</stp>
+        <stp>BDH|3378715445201000261</stp>
         <tr r="C3" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|6071504723843525234</stp>
-        <tr r="O3" s="1"/>
+        <stp>BDH|8441293008358033137</stp>
+        <tr r="S3" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|3480208863472879491</stp>
-        <tr r="AC3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|6459364492508600783</stp>
-        <tr r="U3" s="1"/>
+        <stp>BDH|748707264409896466</stp>
+        <tr r="K3" s="1"/>
       </tp>
     </main>
   </volType>
@@ -604,7 +604,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C29AF7D-B1A9-49E9-BA39-A29DFADF836F}">
-  <dimension ref="A1:AD731"/>
+  <dimension ref="A1:AD751"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -770,105 +770,105 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f>_xll.BDH(B$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=729")</f>
+        <f>_xll.BDH(B$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
         <v>43398</v>
       </c>
       <c r="B3" s="2">
         <v>1.44</v>
       </c>
       <c r="C3" s="1">
-        <f>_xll.BDH(D$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=727")</f>
+        <f>_xll.BDH(D$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=747")</f>
         <v>43398</v>
       </c>
       <c r="D3" s="2">
         <v>1.3774999999999999</v>
       </c>
       <c r="E3" s="1">
-        <f>_xll.BDH(F$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=729")</f>
+        <f>_xll.BDH(F$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
         <v>43398</v>
       </c>
       <c r="F3" s="2">
         <v>1.3674999999999999</v>
       </c>
       <c r="G3" s="1">
-        <f>_xll.BDH(H$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=729")</f>
+        <f>_xll.BDH(H$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
         <v>43398</v>
       </c>
       <c r="H3" s="2">
         <v>1.3774999999999999</v>
       </c>
       <c r="I3" s="1">
-        <f>_xll.BDH(J$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=729")</f>
+        <f>_xll.BDH(J$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
         <v>43398</v>
       </c>
       <c r="J3" s="2">
         <v>1.4</v>
       </c>
       <c r="K3" s="1">
-        <f>_xll.BDH(L$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=729")</f>
+        <f>_xll.BDH(L$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
         <v>43398</v>
       </c>
       <c r="L3" s="2">
         <v>1.4224999999999999</v>
       </c>
       <c r="M3" s="1">
-        <f>_xll.BDH(N$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=729")</f>
+        <f>_xll.BDH(N$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
         <v>43398</v>
       </c>
       <c r="N3" s="2">
         <v>1.4475</v>
       </c>
       <c r="O3" s="1">
-        <f>_xll.BDH(P$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=729")</f>
+        <f>_xll.BDH(P$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
         <v>43398</v>
       </c>
       <c r="P3" s="2">
         <v>1.4750000000000001</v>
       </c>
       <c r="Q3" s="1">
-        <f>_xll.BDH(R$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=729")</f>
+        <f>_xll.BDH(R$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
         <v>43398</v>
       </c>
       <c r="R3" s="2">
         <v>1.5024999999999999</v>
       </c>
       <c r="S3" s="1">
-        <f>_xll.BDH(T$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=729")</f>
+        <f>_xll.BDH(T$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
         <v>43398</v>
       </c>
       <c r="T3" s="2">
         <v>1.5325</v>
       </c>
       <c r="U3" s="1">
-        <f>_xll.BDH(V$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=729")</f>
+        <f>_xll.BDH(V$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
         <v>43398</v>
       </c>
       <c r="V3" s="2">
         <v>1.585</v>
       </c>
       <c r="W3" s="1">
-        <f>_xll.BDH(X$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=729")</f>
+        <f>_xll.BDH(X$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
         <v>43398</v>
       </c>
       <c r="X3" s="2">
         <v>1.67</v>
       </c>
       <c r="Y3" s="1">
-        <f>_xll.BDH(Z$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=729")</f>
+        <f>_xll.BDH(Z$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
         <v>43398</v>
       </c>
       <c r="Z3" s="2">
         <v>1.7850000000000001</v>
       </c>
       <c r="AA3" s="1">
-        <f>_xll.BDH(AB$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=729")</f>
+        <f>_xll.BDH(AB$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
         <v>43398</v>
       </c>
       <c r="AB3" s="2">
         <v>1.87</v>
       </c>
       <c r="AC3" s="1">
-        <f>_xll.BDH(AD$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=729")</f>
+        <f>_xll.BDH(AD$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
         <v>43398</v>
       </c>
       <c r="AD3" s="2">
@@ -67674,6 +67674,12 @@
       <c r="B730">
         <v>1.9424999999999999</v>
       </c>
+      <c r="C730" s="3">
+        <v>44419</v>
+      </c>
+      <c r="D730">
+        <v>1.6675</v>
+      </c>
       <c r="E730" s="3">
         <v>44417</v>
       </c>
@@ -67760,6 +67766,12 @@
       <c r="B731">
         <v>1.99</v>
       </c>
+      <c r="C731" s="3">
+        <v>44420</v>
+      </c>
+      <c r="D731">
+        <v>1.6875</v>
+      </c>
       <c r="E731" s="3">
         <v>44418</v>
       </c>
@@ -67837,6 +67849,1834 @@
       </c>
       <c r="AD731">
         <v>1.8625</v>
+      </c>
+    </row>
+    <row r="732" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A732" s="3">
+        <v>44419</v>
+      </c>
+      <c r="B732">
+        <v>1.9950000000000001</v>
+      </c>
+      <c r="C732" s="3">
+        <v>44421</v>
+      </c>
+      <c r="D732">
+        <v>1.6924999999999999</v>
+      </c>
+      <c r="E732" s="3">
+        <v>44419</v>
+      </c>
+      <c r="F732">
+        <v>1.5975000000000001</v>
+      </c>
+      <c r="G732" s="3">
+        <v>44419</v>
+      </c>
+      <c r="H732">
+        <v>1.585</v>
+      </c>
+      <c r="I732" s="3">
+        <v>44419</v>
+      </c>
+      <c r="J732">
+        <v>1.6025</v>
+      </c>
+      <c r="K732" s="3">
+        <v>44419</v>
+      </c>
+      <c r="L732">
+        <v>1.6175000000000002</v>
+      </c>
+      <c r="M732" s="3">
+        <v>44419</v>
+      </c>
+      <c r="N732">
+        <v>1.63</v>
+      </c>
+      <c r="O732" s="3">
+        <v>44419</v>
+      </c>
+      <c r="P732">
+        <v>1.635</v>
+      </c>
+      <c r="Q732" s="3">
+        <v>44419</v>
+      </c>
+      <c r="R732">
+        <v>1.6400000000000001</v>
+      </c>
+      <c r="S732" s="3">
+        <v>44419</v>
+      </c>
+      <c r="T732">
+        <v>1.65</v>
+      </c>
+      <c r="U732" s="3">
+        <v>44419</v>
+      </c>
+      <c r="V732">
+        <v>1.6825000000000001</v>
+      </c>
+      <c r="W732" s="3">
+        <v>44419</v>
+      </c>
+      <c r="X732">
+        <v>1.7425000000000002</v>
+      </c>
+      <c r="Y732" s="3">
+        <v>44419</v>
+      </c>
+      <c r="Z732">
+        <v>1.8075000000000001</v>
+      </c>
+      <c r="AA732" s="3">
+        <v>44419</v>
+      </c>
+      <c r="AB732">
+        <v>1.8475000000000001</v>
+      </c>
+      <c r="AC732" s="3">
+        <v>44419</v>
+      </c>
+      <c r="AD732">
+        <v>1.8774999999999999</v>
+      </c>
+    </row>
+    <row r="733" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A733" s="3">
+        <v>44420</v>
+      </c>
+      <c r="B733">
+        <v>2.0074999999999998</v>
+      </c>
+      <c r="C733" s="3">
+        <v>44424</v>
+      </c>
+      <c r="D733">
+        <v>1.6875</v>
+      </c>
+      <c r="E733" s="3">
+        <v>44420</v>
+      </c>
+      <c r="F733">
+        <v>1.62</v>
+      </c>
+      <c r="G733" s="3">
+        <v>44420</v>
+      </c>
+      <c r="H733">
+        <v>1.6074999999999999</v>
+      </c>
+      <c r="I733" s="3">
+        <v>44420</v>
+      </c>
+      <c r="J733">
+        <v>1.625</v>
+      </c>
+      <c r="K733" s="3">
+        <v>44420</v>
+      </c>
+      <c r="L733">
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="M733" s="3">
+        <v>44420</v>
+      </c>
+      <c r="N733">
+        <v>1.65</v>
+      </c>
+      <c r="O733" s="3">
+        <v>44420</v>
+      </c>
+      <c r="P733">
+        <v>1.655</v>
+      </c>
+      <c r="Q733" s="3">
+        <v>44420</v>
+      </c>
+      <c r="R733">
+        <v>1.6600000000000001</v>
+      </c>
+      <c r="S733" s="3">
+        <v>44420</v>
+      </c>
+      <c r="T733">
+        <v>1.67</v>
+      </c>
+      <c r="U733" s="3">
+        <v>44420</v>
+      </c>
+      <c r="V733">
+        <v>1.7</v>
+      </c>
+      <c r="W733" s="3">
+        <v>44420</v>
+      </c>
+      <c r="X733">
+        <v>1.76</v>
+      </c>
+      <c r="Y733" s="3">
+        <v>44420</v>
+      </c>
+      <c r="Z733">
+        <v>1.8275000000000001</v>
+      </c>
+      <c r="AA733" s="3">
+        <v>44420</v>
+      </c>
+      <c r="AB733">
+        <v>1.8675000000000002</v>
+      </c>
+      <c r="AC733" s="3">
+        <v>44420</v>
+      </c>
+      <c r="AD733">
+        <v>1.895</v>
+      </c>
+    </row>
+    <row r="734" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A734" s="3">
+        <v>44421</v>
+      </c>
+      <c r="B734">
+        <v>2.02</v>
+      </c>
+      <c r="C734" s="3">
+        <v>44425</v>
+      </c>
+      <c r="D734">
+        <v>1.6975</v>
+      </c>
+      <c r="E734" s="3">
+        <v>44421</v>
+      </c>
+      <c r="F734">
+        <v>1.625</v>
+      </c>
+      <c r="G734" s="3">
+        <v>44421</v>
+      </c>
+      <c r="H734">
+        <v>1.615</v>
+      </c>
+      <c r="I734" s="3">
+        <v>44421</v>
+      </c>
+      <c r="J734">
+        <v>1.6274999999999999</v>
+      </c>
+      <c r="K734" s="3">
+        <v>44421</v>
+      </c>
+      <c r="L734">
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="M734" s="3">
+        <v>44421</v>
+      </c>
+      <c r="N734">
+        <v>1.65</v>
+      </c>
+      <c r="O734" s="3">
+        <v>44421</v>
+      </c>
+      <c r="P734">
+        <v>1.6524999999999999</v>
+      </c>
+      <c r="Q734" s="3">
+        <v>44421</v>
+      </c>
+      <c r="R734">
+        <v>1.655</v>
+      </c>
+      <c r="S734" s="3">
+        <v>44421</v>
+      </c>
+      <c r="T734">
+        <v>1.665</v>
+      </c>
+      <c r="U734" s="3">
+        <v>44421</v>
+      </c>
+      <c r="V734">
+        <v>1.6949999999999998</v>
+      </c>
+      <c r="W734" s="3">
+        <v>44421</v>
+      </c>
+      <c r="X734">
+        <v>1.7549999999999999</v>
+      </c>
+      <c r="Y734" s="3">
+        <v>44421</v>
+      </c>
+      <c r="Z734">
+        <v>1.8225</v>
+      </c>
+      <c r="AA734" s="3">
+        <v>44421</v>
+      </c>
+      <c r="AB734">
+        <v>1.8625</v>
+      </c>
+      <c r="AC734" s="3">
+        <v>44421</v>
+      </c>
+      <c r="AD734">
+        <v>1.8900000000000001</v>
+      </c>
+    </row>
+    <row r="735" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A735" s="3">
+        <v>44424</v>
+      </c>
+      <c r="B735">
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="C735" s="3">
+        <v>44426</v>
+      </c>
+      <c r="D735">
+        <v>1.7025000000000001</v>
+      </c>
+      <c r="E735" s="3">
+        <v>44424</v>
+      </c>
+      <c r="F735">
+        <v>1.615</v>
+      </c>
+      <c r="G735" s="3">
+        <v>44424</v>
+      </c>
+      <c r="H735">
+        <v>1.6025</v>
+      </c>
+      <c r="I735" s="3">
+        <v>44424</v>
+      </c>
+      <c r="J735">
+        <v>1.6125</v>
+      </c>
+      <c r="K735" s="3">
+        <v>44424</v>
+      </c>
+      <c r="L735">
+        <v>1.6274999999999999</v>
+      </c>
+      <c r="M735" s="3">
+        <v>44424</v>
+      </c>
+      <c r="N735">
+        <v>1.6324999999999998</v>
+      </c>
+      <c r="O735" s="3">
+        <v>44424</v>
+      </c>
+      <c r="P735">
+        <v>1.6375</v>
+      </c>
+      <c r="Q735" s="3">
+        <v>44424</v>
+      </c>
+      <c r="R735">
+        <v>1.6400000000000001</v>
+      </c>
+      <c r="S735" s="3">
+        <v>44424</v>
+      </c>
+      <c r="T735">
+        <v>1.6475</v>
+      </c>
+      <c r="U735" s="3">
+        <v>44424</v>
+      </c>
+      <c r="V735">
+        <v>1.6775</v>
+      </c>
+      <c r="W735" s="3">
+        <v>44424</v>
+      </c>
+      <c r="X735">
+        <v>1.74</v>
+      </c>
+      <c r="Y735" s="3">
+        <v>44424</v>
+      </c>
+      <c r="Z735">
+        <v>1.8075000000000001</v>
+      </c>
+      <c r="AA735" s="3">
+        <v>44424</v>
+      </c>
+      <c r="AB735">
+        <v>1.8475000000000001</v>
+      </c>
+      <c r="AC735" s="3">
+        <v>44424</v>
+      </c>
+      <c r="AD735">
+        <v>1.8774999999999999</v>
+      </c>
+    </row>
+    <row r="736" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A736" s="3">
+        <v>44425</v>
+      </c>
+      <c r="B736">
+        <v>2.02</v>
+      </c>
+      <c r="C736" s="3">
+        <v>44427</v>
+      </c>
+      <c r="D736">
+        <v>1.6825000000000001</v>
+      </c>
+      <c r="E736" s="3">
+        <v>44425</v>
+      </c>
+      <c r="F736">
+        <v>1.62</v>
+      </c>
+      <c r="G736" s="3">
+        <v>44425</v>
+      </c>
+      <c r="H736">
+        <v>1.605</v>
+      </c>
+      <c r="I736" s="3">
+        <v>44425</v>
+      </c>
+      <c r="J736">
+        <v>1.6125</v>
+      </c>
+      <c r="K736" s="3">
+        <v>44425</v>
+      </c>
+      <c r="L736">
+        <v>1.625</v>
+      </c>
+      <c r="M736" s="3">
+        <v>44425</v>
+      </c>
+      <c r="N736">
+        <v>1.6324999999999998</v>
+      </c>
+      <c r="O736" s="3">
+        <v>44425</v>
+      </c>
+      <c r="P736">
+        <v>1.6375</v>
+      </c>
+      <c r="Q736" s="3">
+        <v>44425</v>
+      </c>
+      <c r="R736">
+        <v>1.6375</v>
+      </c>
+      <c r="S736" s="3">
+        <v>44425</v>
+      </c>
+      <c r="T736">
+        <v>1.645</v>
+      </c>
+      <c r="U736" s="3">
+        <v>44425</v>
+      </c>
+      <c r="V736">
+        <v>1.675</v>
+      </c>
+      <c r="W736" s="3">
+        <v>44425</v>
+      </c>
+      <c r="X736">
+        <v>1.7375</v>
+      </c>
+      <c r="Y736" s="3">
+        <v>44425</v>
+      </c>
+      <c r="Z736">
+        <v>1.8025</v>
+      </c>
+      <c r="AA736" s="3">
+        <v>44425</v>
+      </c>
+      <c r="AB736">
+        <v>1.8425</v>
+      </c>
+      <c r="AC736" s="3">
+        <v>44425</v>
+      </c>
+      <c r="AD736">
+        <v>1.8725000000000001</v>
+      </c>
+    </row>
+    <row r="737" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A737" s="3">
+        <v>44426</v>
+      </c>
+      <c r="B737">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="C737" s="3">
+        <v>44428</v>
+      </c>
+      <c r="D737">
+        <v>1.6524999999999999</v>
+      </c>
+      <c r="E737" s="3">
+        <v>44426</v>
+      </c>
+      <c r="F737">
+        <v>1.62</v>
+      </c>
+      <c r="G737" s="3">
+        <v>44426</v>
+      </c>
+      <c r="H737">
+        <v>1.6025</v>
+      </c>
+      <c r="I737" s="3">
+        <v>44426</v>
+      </c>
+      <c r="J737">
+        <v>1.6074999999999999</v>
+      </c>
+      <c r="K737" s="3">
+        <v>44426</v>
+      </c>
+      <c r="L737">
+        <v>1.62</v>
+      </c>
+      <c r="M737" s="3">
+        <v>44426</v>
+      </c>
+      <c r="N737">
+        <v>1.625</v>
+      </c>
+      <c r="O737" s="3">
+        <v>44426</v>
+      </c>
+      <c r="P737">
+        <v>1.63</v>
+      </c>
+      <c r="Q737" s="3">
+        <v>44426</v>
+      </c>
+      <c r="R737">
+        <v>1.6274999999999999</v>
+      </c>
+      <c r="S737" s="3">
+        <v>44426</v>
+      </c>
+      <c r="T737">
+        <v>1.6375</v>
+      </c>
+      <c r="U737" s="3">
+        <v>44426</v>
+      </c>
+      <c r="V737">
+        <v>1.6675</v>
+      </c>
+      <c r="W737" s="3">
+        <v>44426</v>
+      </c>
+      <c r="X737">
+        <v>1.7275</v>
+      </c>
+      <c r="Y737" s="3">
+        <v>44426</v>
+      </c>
+      <c r="Z737">
+        <v>1.7925</v>
+      </c>
+      <c r="AA737" s="3">
+        <v>44426</v>
+      </c>
+      <c r="AB737">
+        <v>1.8325</v>
+      </c>
+      <c r="AC737" s="3">
+        <v>44426</v>
+      </c>
+      <c r="AD737">
+        <v>1.8625</v>
+      </c>
+    </row>
+    <row r="738" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A738" s="3">
+        <v>44427</v>
+      </c>
+      <c r="B738">
+        <v>1.9975000000000001</v>
+      </c>
+      <c r="C738" s="3">
+        <v>44431</v>
+      </c>
+      <c r="D738">
+        <v>1.6924999999999999</v>
+      </c>
+      <c r="E738" s="3">
+        <v>44427</v>
+      </c>
+      <c r="F738">
+        <v>1.6</v>
+      </c>
+      <c r="G738" s="3">
+        <v>44427</v>
+      </c>
+      <c r="H738">
+        <v>1.5825</v>
+      </c>
+      <c r="I738" s="3">
+        <v>44427</v>
+      </c>
+      <c r="J738">
+        <v>1.5874999999999999</v>
+      </c>
+      <c r="K738" s="3">
+        <v>44427</v>
+      </c>
+      <c r="L738">
+        <v>1.6</v>
+      </c>
+      <c r="M738" s="3">
+        <v>44427</v>
+      </c>
+      <c r="N738">
+        <v>1.605</v>
+      </c>
+      <c r="O738" s="3">
+        <v>44427</v>
+      </c>
+      <c r="P738">
+        <v>1.6099999999999999</v>
+      </c>
+      <c r="Q738" s="3">
+        <v>44427</v>
+      </c>
+      <c r="R738">
+        <v>1.6074999999999999</v>
+      </c>
+      <c r="S738" s="3">
+        <v>44427</v>
+      </c>
+      <c r="T738">
+        <v>1.6175000000000002</v>
+      </c>
+      <c r="U738" s="3">
+        <v>44427</v>
+      </c>
+      <c r="V738">
+        <v>1.6475</v>
+      </c>
+      <c r="W738" s="3">
+        <v>44427</v>
+      </c>
+      <c r="X738">
+        <v>1.71</v>
+      </c>
+      <c r="Y738" s="3">
+        <v>44427</v>
+      </c>
+      <c r="Z738">
+        <v>1.7749999999999999</v>
+      </c>
+      <c r="AA738" s="3">
+        <v>44427</v>
+      </c>
+      <c r="AB738">
+        <v>1.8174999999999999</v>
+      </c>
+      <c r="AC738" s="3">
+        <v>44427</v>
+      </c>
+      <c r="AD738">
+        <v>1.845</v>
+      </c>
+    </row>
+    <row r="739" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A739" s="3">
+        <v>44428</v>
+      </c>
+      <c r="B739">
+        <v>1.9675</v>
+      </c>
+      <c r="C739" s="3">
+        <v>44432</v>
+      </c>
+      <c r="D739">
+        <v>1.72</v>
+      </c>
+      <c r="E739" s="3">
+        <v>44428</v>
+      </c>
+      <c r="F739">
+        <v>1.5775000000000001</v>
+      </c>
+      <c r="G739" s="3">
+        <v>44428</v>
+      </c>
+      <c r="H739">
+        <v>1.56</v>
+      </c>
+      <c r="I739" s="3">
+        <v>44428</v>
+      </c>
+      <c r="J739">
+        <v>1.5674999999999999</v>
+      </c>
+      <c r="K739" s="3">
+        <v>44428</v>
+      </c>
+      <c r="L739">
+        <v>1.5825</v>
+      </c>
+      <c r="M739" s="3">
+        <v>44428</v>
+      </c>
+      <c r="N739">
+        <v>1.5899999999999999</v>
+      </c>
+      <c r="O739" s="3">
+        <v>44428</v>
+      </c>
+      <c r="P739">
+        <v>1.5975000000000001</v>
+      </c>
+      <c r="Q739" s="3">
+        <v>44428</v>
+      </c>
+      <c r="R739">
+        <v>1.5975000000000001</v>
+      </c>
+      <c r="S739" s="3">
+        <v>44428</v>
+      </c>
+      <c r="T739">
+        <v>1.6074999999999999</v>
+      </c>
+      <c r="U739" s="3">
+        <v>44428</v>
+      </c>
+      <c r="V739">
+        <v>1.6375</v>
+      </c>
+      <c r="W739" s="3">
+        <v>44428</v>
+      </c>
+      <c r="X739">
+        <v>1.7</v>
+      </c>
+      <c r="Y739" s="3">
+        <v>44428</v>
+      </c>
+      <c r="Z739">
+        <v>1.7675000000000001</v>
+      </c>
+      <c r="AA739" s="3">
+        <v>44428</v>
+      </c>
+      <c r="AB739">
+        <v>1.8075000000000001</v>
+      </c>
+      <c r="AC739" s="3">
+        <v>44428</v>
+      </c>
+      <c r="AD739">
+        <v>1.8374999999999999</v>
+      </c>
+    </row>
+    <row r="740" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A740" s="3">
+        <v>44431</v>
+      </c>
+      <c r="B740">
+        <v>2.0150000000000001</v>
+      </c>
+      <c r="C740" s="3">
+        <v>44433</v>
+      </c>
+      <c r="D740">
+        <v>1.76</v>
+      </c>
+      <c r="E740" s="3">
+        <v>44431</v>
+      </c>
+      <c r="F740">
+        <v>1.6125</v>
+      </c>
+      <c r="G740" s="3">
+        <v>44431</v>
+      </c>
+      <c r="H740">
+        <v>1.5925</v>
+      </c>
+      <c r="I740" s="3">
+        <v>44431</v>
+      </c>
+      <c r="J740">
+        <v>1.595</v>
+      </c>
+      <c r="K740" s="3">
+        <v>44431</v>
+      </c>
+      <c r="L740">
+        <v>1.6074999999999999</v>
+      </c>
+      <c r="M740" s="3">
+        <v>44431</v>
+      </c>
+      <c r="N740">
+        <v>1.615</v>
+      </c>
+      <c r="O740" s="3">
+        <v>44431</v>
+      </c>
+      <c r="P740">
+        <v>1.615</v>
+      </c>
+      <c r="Q740" s="3">
+        <v>44431</v>
+      </c>
+      <c r="R740">
+        <v>1.62</v>
+      </c>
+      <c r="S740" s="3">
+        <v>44431</v>
+      </c>
+      <c r="T740">
+        <v>1.6274999999999999</v>
+      </c>
+      <c r="U740" s="3">
+        <v>44431</v>
+      </c>
+      <c r="V740">
+        <v>1.6575</v>
+      </c>
+      <c r="W740" s="3">
+        <v>44431</v>
+      </c>
+      <c r="X740">
+        <v>1.7175</v>
+      </c>
+      <c r="Y740" s="3">
+        <v>44431</v>
+      </c>
+      <c r="Z740">
+        <v>1.7850000000000001</v>
+      </c>
+      <c r="AA740" s="3">
+        <v>44431</v>
+      </c>
+      <c r="AB740">
+        <v>1.8225</v>
+      </c>
+      <c r="AC740" s="3">
+        <v>44431</v>
+      </c>
+      <c r="AD740">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="741" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A741" s="3">
+        <v>44432</v>
+      </c>
+      <c r="B741">
+        <v>2.0449999999999999</v>
+      </c>
+      <c r="C741" s="3">
+        <v>44434</v>
+      </c>
+      <c r="D741">
+        <v>1.7275</v>
+      </c>
+      <c r="E741" s="3">
+        <v>44432</v>
+      </c>
+      <c r="F741">
+        <v>1.6375</v>
+      </c>
+      <c r="G741" s="3">
+        <v>44432</v>
+      </c>
+      <c r="H741">
+        <v>1.6175000000000002</v>
+      </c>
+      <c r="I741" s="3">
+        <v>44432</v>
+      </c>
+      <c r="J741">
+        <v>1.615</v>
+      </c>
+      <c r="K741" s="3">
+        <v>44432</v>
+      </c>
+      <c r="L741">
+        <v>1.62</v>
+      </c>
+      <c r="M741" s="3">
+        <v>44432</v>
+      </c>
+      <c r="N741">
+        <v>1.6274999999999999</v>
+      </c>
+      <c r="O741" s="3">
+        <v>44432</v>
+      </c>
+      <c r="P741">
+        <v>1.63</v>
+      </c>
+      <c r="Q741" s="3">
+        <v>44432</v>
+      </c>
+      <c r="R741">
+        <v>1.6324999999999998</v>
+      </c>
+      <c r="S741" s="3">
+        <v>44432</v>
+      </c>
+      <c r="T741">
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="U741" s="3">
+        <v>44432</v>
+      </c>
+      <c r="V741">
+        <v>1.6724999999999999</v>
+      </c>
+      <c r="W741" s="3">
+        <v>44432</v>
+      </c>
+      <c r="X741">
+        <v>1.7324999999999999</v>
+      </c>
+      <c r="Y741" s="3">
+        <v>44432</v>
+      </c>
+      <c r="Z741">
+        <v>1.7974999999999999</v>
+      </c>
+      <c r="AA741" s="3">
+        <v>44432</v>
+      </c>
+      <c r="AB741">
+        <v>1.8374999999999999</v>
+      </c>
+      <c r="AC741" s="3">
+        <v>44432</v>
+      </c>
+      <c r="AD741">
+        <v>1.8675000000000002</v>
+      </c>
+    </row>
+    <row r="742" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A742" s="3">
+        <v>44433</v>
+      </c>
+      <c r="B742">
+        <v>2.105</v>
+      </c>
+      <c r="C742" s="3">
+        <v>44435</v>
+      </c>
+      <c r="D742">
+        <v>1.7425000000000002</v>
+      </c>
+      <c r="E742" s="3">
+        <v>44433</v>
+      </c>
+      <c r="F742">
+        <v>1.6724999999999999</v>
+      </c>
+      <c r="G742" s="3">
+        <v>44433</v>
+      </c>
+      <c r="H742">
+        <v>1.6475</v>
+      </c>
+      <c r="I742" s="3">
+        <v>44433</v>
+      </c>
+      <c r="J742">
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="K742" s="3">
+        <v>44433</v>
+      </c>
+      <c r="L742">
+        <v>1.645</v>
+      </c>
+      <c r="M742" s="3">
+        <v>44433</v>
+      </c>
+      <c r="N742">
+        <v>1.6524999999999999</v>
+      </c>
+      <c r="O742" s="3">
+        <v>44433</v>
+      </c>
+      <c r="P742">
+        <v>1.655</v>
+      </c>
+      <c r="Q742" s="3">
+        <v>44433</v>
+      </c>
+      <c r="R742">
+        <v>1.6600000000000001</v>
+      </c>
+      <c r="S742" s="3">
+        <v>44433</v>
+      </c>
+      <c r="T742">
+        <v>1.67</v>
+      </c>
+      <c r="U742" s="3">
+        <v>44433</v>
+      </c>
+      <c r="V742">
+        <v>1.7</v>
+      </c>
+      <c r="W742" s="3">
+        <v>44433</v>
+      </c>
+      <c r="X742">
+        <v>1.76</v>
+      </c>
+      <c r="Y742" s="3">
+        <v>44433</v>
+      </c>
+      <c r="Z742">
+        <v>1.825</v>
+      </c>
+      <c r="AA742" s="3">
+        <v>44433</v>
+      </c>
+      <c r="AB742">
+        <v>1.865</v>
+      </c>
+      <c r="AC742" s="3">
+        <v>44433</v>
+      </c>
+      <c r="AD742">
+        <v>1.8925000000000001</v>
+      </c>
+    </row>
+    <row r="743" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A743" s="3">
+        <v>44434</v>
+      </c>
+      <c r="B743">
+        <v>2.09</v>
+      </c>
+      <c r="C743" s="3">
+        <v>44438</v>
+      </c>
+      <c r="D743">
+        <v>1.7450000000000001</v>
+      </c>
+      <c r="E743" s="3">
+        <v>44434</v>
+      </c>
+      <c r="F743">
+        <v>1.645</v>
+      </c>
+      <c r="G743" s="3">
+        <v>44434</v>
+      </c>
+      <c r="H743">
+        <v>1.6274999999999999</v>
+      </c>
+      <c r="I743" s="3">
+        <v>44434</v>
+      </c>
+      <c r="J743">
+        <v>1.625</v>
+      </c>
+      <c r="K743" s="3">
+        <v>44434</v>
+      </c>
+      <c r="L743">
+        <v>1.6274999999999999</v>
+      </c>
+      <c r="M743" s="3">
+        <v>44434</v>
+      </c>
+      <c r="N743">
+        <v>1.635</v>
+      </c>
+      <c r="O743" s="3">
+        <v>44434</v>
+      </c>
+      <c r="P743">
+        <v>1.6375</v>
+      </c>
+      <c r="Q743" s="3">
+        <v>44434</v>
+      </c>
+      <c r="R743">
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="S743" s="3">
+        <v>44434</v>
+      </c>
+      <c r="T743">
+        <v>1.6524999999999999</v>
+      </c>
+      <c r="U743" s="3">
+        <v>44434</v>
+      </c>
+      <c r="V743">
+        <v>1.6825000000000001</v>
+      </c>
+      <c r="W743" s="3">
+        <v>44434</v>
+      </c>
+      <c r="X743">
+        <v>1.7450000000000001</v>
+      </c>
+      <c r="Y743" s="3">
+        <v>44434</v>
+      </c>
+      <c r="Z743">
+        <v>1.8125</v>
+      </c>
+      <c r="AA743" s="3">
+        <v>44434</v>
+      </c>
+      <c r="AB743">
+        <v>1.855</v>
+      </c>
+      <c r="AC743" s="3">
+        <v>44434</v>
+      </c>
+      <c r="AD743">
+        <v>1.885</v>
+      </c>
+    </row>
+    <row r="744" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A744" s="3">
+        <v>44435</v>
+      </c>
+      <c r="B744">
+        <v>2.14</v>
+      </c>
+      <c r="C744" s="3">
+        <v>44439</v>
+      </c>
+      <c r="D744">
+        <v>1.8075000000000001</v>
+      </c>
+      <c r="E744" s="3">
+        <v>44435</v>
+      </c>
+      <c r="F744">
+        <v>1.6575</v>
+      </c>
+      <c r="G744" s="3">
+        <v>44435</v>
+      </c>
+      <c r="H744">
+        <v>1.6375</v>
+      </c>
+      <c r="I744" s="3">
+        <v>44435</v>
+      </c>
+      <c r="J744">
+        <v>1.635</v>
+      </c>
+      <c r="K744" s="3">
+        <v>44435</v>
+      </c>
+      <c r="L744">
+        <v>1.6375</v>
+      </c>
+      <c r="M744" s="3">
+        <v>44435</v>
+      </c>
+      <c r="N744">
+        <v>1.645</v>
+      </c>
+      <c r="O744" s="3">
+        <v>44435</v>
+      </c>
+      <c r="P744">
+        <v>1.65</v>
+      </c>
+      <c r="Q744" s="3">
+        <v>44435</v>
+      </c>
+      <c r="R744">
+        <v>1.655</v>
+      </c>
+      <c r="S744" s="3">
+        <v>44435</v>
+      </c>
+      <c r="T744">
+        <v>1.665</v>
+      </c>
+      <c r="U744" s="3">
+        <v>44435</v>
+      </c>
+      <c r="V744">
+        <v>1.6949999999999998</v>
+      </c>
+      <c r="W744" s="3">
+        <v>44435</v>
+      </c>
+      <c r="X744">
+        <v>1.7574999999999998</v>
+      </c>
+      <c r="Y744" s="3">
+        <v>44435</v>
+      </c>
+      <c r="Z744">
+        <v>1.825</v>
+      </c>
+      <c r="AA744" s="3">
+        <v>44435</v>
+      </c>
+      <c r="AB744">
+        <v>1.8675000000000002</v>
+      </c>
+      <c r="AC744" s="3">
+        <v>44435</v>
+      </c>
+      <c r="AD744">
+        <v>1.895</v>
+      </c>
+    </row>
+    <row r="745" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A745" s="3">
+        <v>44438</v>
+      </c>
+      <c r="B745">
+        <v>2.1425000000000001</v>
+      </c>
+      <c r="C745" s="3">
+        <v>44440</v>
+      </c>
+      <c r="D745">
+        <v>1.7450000000000001</v>
+      </c>
+      <c r="E745" s="3">
+        <v>44438</v>
+      </c>
+      <c r="F745">
+        <v>1.6600000000000001</v>
+      </c>
+      <c r="G745" s="3">
+        <v>44438</v>
+      </c>
+      <c r="H745">
+        <v>1.6400000000000001</v>
+      </c>
+      <c r="I745" s="3">
+        <v>44438</v>
+      </c>
+      <c r="J745">
+        <v>1.6375</v>
+      </c>
+      <c r="K745" s="3">
+        <v>44438</v>
+      </c>
+      <c r="L745">
+        <v>1.6400000000000001</v>
+      </c>
+      <c r="M745" s="3">
+        <v>44438</v>
+      </c>
+      <c r="N745">
+        <v>1.6475</v>
+      </c>
+      <c r="O745" s="3">
+        <v>44438</v>
+      </c>
+      <c r="P745">
+        <v>1.6524999999999999</v>
+      </c>
+      <c r="Q745" s="3">
+        <v>44438</v>
+      </c>
+      <c r="R745">
+        <v>1.6575</v>
+      </c>
+      <c r="S745" s="3">
+        <v>44438</v>
+      </c>
+      <c r="T745">
+        <v>1.665</v>
+      </c>
+      <c r="U745" s="3">
+        <v>44438</v>
+      </c>
+      <c r="V745">
+        <v>1.6924999999999999</v>
+      </c>
+      <c r="W745" s="3">
+        <v>44438</v>
+      </c>
+      <c r="X745">
+        <v>1.7549999999999999</v>
+      </c>
+      <c r="Y745" s="3">
+        <v>44438</v>
+      </c>
+      <c r="Z745">
+        <v>1.8199999999999998</v>
+      </c>
+      <c r="AA745" s="3">
+        <v>44438</v>
+      </c>
+      <c r="AB745">
+        <v>1.8625</v>
+      </c>
+      <c r="AC745" s="3">
+        <v>44438</v>
+      </c>
+      <c r="AD745">
+        <v>1.8900000000000001</v>
+      </c>
+    </row>
+    <row r="746" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A746" s="3">
+        <v>44439</v>
+      </c>
+      <c r="B746">
+        <v>2.2650000000000001</v>
+      </c>
+      <c r="C746" s="3">
+        <v>44441</v>
+      </c>
+      <c r="D746">
+        <v>1.79</v>
+      </c>
+      <c r="E746" s="3">
+        <v>44439</v>
+      </c>
+      <c r="F746">
+        <v>1.71</v>
+      </c>
+      <c r="G746" s="3">
+        <v>44439</v>
+      </c>
+      <c r="H746">
+        <v>1.6775</v>
+      </c>
+      <c r="I746" s="3">
+        <v>44439</v>
+      </c>
+      <c r="J746">
+        <v>1.665</v>
+      </c>
+      <c r="K746" s="3">
+        <v>44439</v>
+      </c>
+      <c r="L746">
+        <v>1.6625000000000001</v>
+      </c>
+      <c r="M746" s="3">
+        <v>44439</v>
+      </c>
+      <c r="N746">
+        <v>1.665</v>
+      </c>
+      <c r="O746" s="3">
+        <v>44439</v>
+      </c>
+      <c r="P746">
+        <v>1.665</v>
+      </c>
+      <c r="Q746" s="3">
+        <v>44439</v>
+      </c>
+      <c r="R746">
+        <v>1.6675</v>
+      </c>
+      <c r="S746" s="3">
+        <v>44439</v>
+      </c>
+      <c r="T746">
+        <v>1.675</v>
+      </c>
+      <c r="U746" s="3">
+        <v>44439</v>
+      </c>
+      <c r="V746">
+        <v>1.7025000000000001</v>
+      </c>
+      <c r="W746" s="3">
+        <v>44439</v>
+      </c>
+      <c r="X746">
+        <v>1.7650000000000001</v>
+      </c>
+      <c r="Y746" s="3">
+        <v>44439</v>
+      </c>
+      <c r="Z746">
+        <v>1.83</v>
+      </c>
+      <c r="AA746" s="3">
+        <v>44439</v>
+      </c>
+      <c r="AB746">
+        <v>1.8725000000000001</v>
+      </c>
+      <c r="AC746" s="3">
+        <v>44439</v>
+      </c>
+      <c r="AD746">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="747" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A747" s="3">
+        <v>44440</v>
+      </c>
+      <c r="B747">
+        <v>2.1850000000000001</v>
+      </c>
+      <c r="C747" s="3">
+        <v>44442</v>
+      </c>
+      <c r="D747">
+        <v>1.8425</v>
+      </c>
+      <c r="E747" s="3">
+        <v>44440</v>
+      </c>
+      <c r="F747">
+        <v>1.6524999999999999</v>
+      </c>
+      <c r="G747" s="3">
+        <v>44440</v>
+      </c>
+      <c r="H747">
+        <v>1.6375</v>
+      </c>
+      <c r="I747" s="3">
+        <v>44440</v>
+      </c>
+      <c r="J747">
+        <v>1.635</v>
+      </c>
+      <c r="K747" s="3">
+        <v>44440</v>
+      </c>
+      <c r="L747">
+        <v>1.6375</v>
+      </c>
+      <c r="M747" s="3">
+        <v>44440</v>
+      </c>
+      <c r="N747">
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="O747" s="3">
+        <v>44440</v>
+      </c>
+      <c r="P747">
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="Q747" s="3">
+        <v>44440</v>
+      </c>
+      <c r="R747">
+        <v>1.6475</v>
+      </c>
+      <c r="S747" s="3">
+        <v>44440</v>
+      </c>
+      <c r="T747">
+        <v>1.6575</v>
+      </c>
+      <c r="U747" s="3">
+        <v>44440</v>
+      </c>
+      <c r="V747">
+        <v>1.6850000000000001</v>
+      </c>
+      <c r="W747" s="3">
+        <v>44440</v>
+      </c>
+      <c r="X747">
+        <v>1.7475000000000001</v>
+      </c>
+      <c r="Y747" s="3">
+        <v>44440</v>
+      </c>
+      <c r="Z747">
+        <v>1.8149999999999999</v>
+      </c>
+      <c r="AA747" s="3">
+        <v>44440</v>
+      </c>
+      <c r="AB747">
+        <v>1.8574999999999999</v>
+      </c>
+      <c r="AC747" s="3">
+        <v>44440</v>
+      </c>
+      <c r="AD747">
+        <v>1.8875</v>
+      </c>
+    </row>
+    <row r="748" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A748" s="3">
+        <v>44441</v>
+      </c>
+      <c r="B748">
+        <v>2.2425000000000002</v>
+      </c>
+      <c r="C748" s="3">
+        <v>44445</v>
+      </c>
+      <c r="D748">
+        <v>1.9275</v>
+      </c>
+      <c r="E748" s="3">
+        <v>44441</v>
+      </c>
+      <c r="F748">
+        <v>1.6850000000000001</v>
+      </c>
+      <c r="G748" s="3">
+        <v>44441</v>
+      </c>
+      <c r="H748">
+        <v>1.6675</v>
+      </c>
+      <c r="I748" s="3">
+        <v>44441</v>
+      </c>
+      <c r="J748">
+        <v>1.6600000000000001</v>
+      </c>
+      <c r="K748" s="3">
+        <v>44441</v>
+      </c>
+      <c r="L748">
+        <v>1.6600000000000001</v>
+      </c>
+      <c r="M748" s="3">
+        <v>44441</v>
+      </c>
+      <c r="N748">
+        <v>1.6625000000000001</v>
+      </c>
+      <c r="O748" s="3">
+        <v>44441</v>
+      </c>
+      <c r="P748">
+        <v>1.6675</v>
+      </c>
+      <c r="Q748" s="3">
+        <v>44441</v>
+      </c>
+      <c r="R748">
+        <v>1.6675</v>
+      </c>
+      <c r="S748" s="3">
+        <v>44441</v>
+      </c>
+      <c r="T748">
+        <v>1.6724999999999999</v>
+      </c>
+      <c r="U748" s="3">
+        <v>44441</v>
+      </c>
+      <c r="V748">
+        <v>1.6949999999999998</v>
+      </c>
+      <c r="W748" s="3">
+        <v>44441</v>
+      </c>
+      <c r="X748">
+        <v>1.7524999999999999</v>
+      </c>
+      <c r="Y748" s="3">
+        <v>44441</v>
+      </c>
+      <c r="Z748">
+        <v>1.8174999999999999</v>
+      </c>
+      <c r="AA748" s="3">
+        <v>44441</v>
+      </c>
+      <c r="AB748">
+        <v>1.8574999999999999</v>
+      </c>
+      <c r="AC748" s="3">
+        <v>44441</v>
+      </c>
+      <c r="AD748">
+        <v>1.885</v>
+      </c>
+    </row>
+    <row r="749" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A749" s="3">
+        <v>44442</v>
+      </c>
+      <c r="B749">
+        <v>2.2949999999999999</v>
+      </c>
+      <c r="C749" s="3">
+        <v>44446</v>
+      </c>
+      <c r="D749">
+        <v>1.925</v>
+      </c>
+      <c r="E749" s="3">
+        <v>44442</v>
+      </c>
+      <c r="F749">
+        <v>1.74</v>
+      </c>
+      <c r="G749" s="3">
+        <v>44442</v>
+      </c>
+      <c r="H749">
+        <v>1.7225000000000001</v>
+      </c>
+      <c r="I749" s="3">
+        <v>44442</v>
+      </c>
+      <c r="J749">
+        <v>1.7149999999999999</v>
+      </c>
+      <c r="K749" s="3">
+        <v>44442</v>
+      </c>
+      <c r="L749">
+        <v>1.71</v>
+      </c>
+      <c r="M749" s="3">
+        <v>44442</v>
+      </c>
+      <c r="N749">
+        <v>1.7075</v>
+      </c>
+      <c r="O749" s="3">
+        <v>44442</v>
+      </c>
+      <c r="P749">
+        <v>1.71</v>
+      </c>
+      <c r="Q749" s="3">
+        <v>44442</v>
+      </c>
+      <c r="R749">
+        <v>1.7075</v>
+      </c>
+      <c r="S749" s="3">
+        <v>44442</v>
+      </c>
+      <c r="T749">
+        <v>1.71</v>
+      </c>
+      <c r="U749" s="3">
+        <v>44442</v>
+      </c>
+      <c r="V749">
+        <v>1.7275</v>
+      </c>
+      <c r="W749" s="3">
+        <v>44442</v>
+      </c>
+      <c r="X749">
+        <v>1.7825</v>
+      </c>
+      <c r="Y749" s="3">
+        <v>44442</v>
+      </c>
+      <c r="Z749">
+        <v>1.8425</v>
+      </c>
+      <c r="AA749" s="3">
+        <v>44442</v>
+      </c>
+      <c r="AB749">
+        <v>1.8824999999999998</v>
+      </c>
+      <c r="AC749" s="3">
+        <v>44442</v>
+      </c>
+      <c r="AD749">
+        <v>1.9075</v>
+      </c>
+    </row>
+    <row r="750" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A750" s="3">
+        <v>44445</v>
+      </c>
+      <c r="B750">
+        <v>2.3875000000000002</v>
+      </c>
+      <c r="E750" s="3">
+        <v>44445</v>
+      </c>
+      <c r="F750">
+        <v>1.8174999999999999</v>
+      </c>
+      <c r="G750" s="3">
+        <v>44445</v>
+      </c>
+      <c r="H750">
+        <v>1.7949999999999999</v>
+      </c>
+      <c r="I750" s="3">
+        <v>44445</v>
+      </c>
+      <c r="J750">
+        <v>1.7774999999999999</v>
+      </c>
+      <c r="K750" s="3">
+        <v>44445</v>
+      </c>
+      <c r="L750">
+        <v>1.77</v>
+      </c>
+      <c r="M750" s="3">
+        <v>44445</v>
+      </c>
+      <c r="N750">
+        <v>1.7650000000000001</v>
+      </c>
+      <c r="O750" s="3">
+        <v>44445</v>
+      </c>
+      <c r="P750">
+        <v>1.7650000000000001</v>
+      </c>
+      <c r="Q750" s="3">
+        <v>44445</v>
+      </c>
+      <c r="R750">
+        <v>1.76</v>
+      </c>
+      <c r="S750" s="3">
+        <v>44445</v>
+      </c>
+      <c r="T750">
+        <v>1.7625</v>
+      </c>
+      <c r="U750" s="3">
+        <v>44445</v>
+      </c>
+      <c r="V750">
+        <v>1.7725</v>
+      </c>
+      <c r="W750" s="3">
+        <v>44445</v>
+      </c>
+      <c r="X750">
+        <v>1.8199999999999998</v>
+      </c>
+      <c r="Y750" s="3">
+        <v>44445</v>
+      </c>
+      <c r="Z750">
+        <v>1.875</v>
+      </c>
+      <c r="AA750" s="3">
+        <v>44445</v>
+      </c>
+      <c r="AB750">
+        <v>1.9125000000000001</v>
+      </c>
+      <c r="AC750" s="3">
+        <v>44445</v>
+      </c>
+      <c r="AD750">
+        <v>1.9350000000000001</v>
+      </c>
+    </row>
+    <row r="751" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A751" s="3">
+        <v>44446</v>
+      </c>
+      <c r="B751">
+        <v>2.37</v>
+      </c>
+      <c r="E751" s="3">
+        <v>44446</v>
+      </c>
+      <c r="F751">
+        <v>1.8149999999999999</v>
+      </c>
+      <c r="G751" s="3">
+        <v>44446</v>
+      </c>
+      <c r="H751">
+        <v>1.7925</v>
+      </c>
+      <c r="I751" s="3">
+        <v>44446</v>
+      </c>
+      <c r="J751">
+        <v>1.7774999999999999</v>
+      </c>
+      <c r="K751" s="3">
+        <v>44446</v>
+      </c>
+      <c r="L751">
+        <v>1.77</v>
+      </c>
+      <c r="M751" s="3">
+        <v>44446</v>
+      </c>
+      <c r="N751">
+        <v>1.7625</v>
+      </c>
+      <c r="O751" s="3">
+        <v>44446</v>
+      </c>
+      <c r="P751">
+        <v>1.7625</v>
+      </c>
+      <c r="Q751" s="3">
+        <v>44446</v>
+      </c>
+      <c r="R751">
+        <v>1.7574999999999998</v>
+      </c>
+      <c r="S751" s="3">
+        <v>44446</v>
+      </c>
+      <c r="T751">
+        <v>1.76</v>
+      </c>
+      <c r="U751" s="3">
+        <v>44446</v>
+      </c>
+      <c r="V751">
+        <v>1.7725</v>
+      </c>
+      <c r="W751" s="3">
+        <v>44446</v>
+      </c>
+      <c r="X751">
+        <v>1.825</v>
+      </c>
+      <c r="Y751" s="3">
+        <v>44446</v>
+      </c>
+      <c r="Z751">
+        <v>1.8774999999999999</v>
+      </c>
+      <c r="AA751" s="3">
+        <v>44446</v>
+      </c>
+      <c r="AB751">
+        <v>1.915</v>
+      </c>
+      <c r="AC751" s="3">
+        <v>44446</v>
+      </c>
+      <c r="AD751">
+        <v>1.94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
migrating local changes and modifying data pulls from BFIL to BFIM on bloomberg, series updated as of 10/15 GSW data
</commit_message>
<xml_diff>
--- a/Input/swaps/eur-inflation-HICPxT-swaps.xlsx
+++ b/Input/swaps/eur-inflation-HICPxT-swaps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\SHARE\cmf\Desi\Rajesh\IIE\Input\swaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28B6FB4-79AD-42B6-8AD2-00F89F0067C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC81646-6411-4342-8D53-C3E40D3C0F09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43B30E9F-8D1A-4EAB-8504-0C8FB3A38EDD}"/>
   </bookViews>
@@ -191,116 +191,116 @@
   <volType type="realTimeData">
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...1846912138</v>
+        <v>#N/A Requesting Data...1176465790</v>
         <stp/>
         <stp>BTODAY|10610048301435813905</stp>
+        <tr r="I3" s="1"/>
+        <tr r="Y3" s="1"/>
         <tr r="W3" s="1"/>
+        <tr r="C3" s="1"/>
+        <tr r="AC3" s="1"/>
         <tr r="O3" s="1"/>
+        <tr r="AA3" s="1"/>
         <tr r="E3" s="1"/>
+        <tr r="A3" s="1"/>
+        <tr r="U3" s="1"/>
         <tr r="G3" s="1"/>
-        <tr r="AC3" s="1"/>
+        <tr r="K3" s="1"/>
+        <tr r="S3" s="1"/>
         <tr r="Q3" s="1"/>
-        <tr r="I3" s="1"/>
-        <tr r="S3" s="1"/>
-        <tr r="K3" s="1"/>
-        <tr r="U3" s="1"/>
-        <tr r="Y3" s="1"/>
         <tr r="M3" s="1"/>
-        <tr r="A3" s="1"/>
-        <tr r="C3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|10170462177688019424</stp>
+        <tr r="O3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|18355129732980966699</stp>
         <tr r="AA3" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|13635314096660805235</stp>
-        <tr r="M3" s="1"/>
+        <stp>BDH|17209798741749626058</stp>
+        <tr r="U3" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|12535776639532594737</stp>
-        <tr r="G3" s="1"/>
+        <stp>BDH|12867482838372833572</stp>
+        <tr r="K3" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|11931716834053685603</stp>
-        <tr r="E3" s="1"/>
+        <stp>BDH|15811008171294592772</stp>
+        <tr r="S3" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|13066307407236801762</stp>
-        <tr r="AA3" s="1"/>
+        <stp>BDH|11539343256611304276</stp>
+        <tr r="AC3" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|11091778390002020832</stp>
-        <tr r="O3" s="1"/>
+        <stp>BDH|16051699650285200425</stp>
+        <tr r="A3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|11270969699516606274</stp>
+        <tr r="E3" s="1"/>
       </tp>
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|7432321582823799209</stp>
+        <stp>BDH|2166326884811156453</stp>
+        <tr r="M3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|5399806486401088839</stp>
+        <tr r="Q3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|9791034645182416090</stp>
+        <tr r="C3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|4441791770148129608</stp>
         <tr r="Y3" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|7949973141835531017</stp>
-        <tr r="I3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|8216579873721617135</stp>
-        <tr r="AC3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|1972534724420298299</stp>
+        <stp>BDH|4486650127540142751</stp>
         <tr r="W3" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|2197307417585166338</stp>
-        <tr r="A3" s="1"/>
+        <stp>BDH|9384827152902508174</stp>
+        <tr r="G3" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|1791991040416734868</stp>
-        <tr r="U3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|4582328516234055112</stp>
-        <tr r="Q3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|3378715445201000261</stp>
-        <tr r="C3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|8441293008358033137</stp>
-        <tr r="S3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|748707264409896466</stp>
-        <tr r="K3" s="1"/>
+        <stp>BDH|7993354558947112541</stp>
+        <tr r="I3" s="1"/>
       </tp>
     </main>
   </volType>
@@ -604,11 +604,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C29AF7D-B1A9-49E9-BA39-A29DFADF836F}">
-  <dimension ref="A1:AD751"/>
+  <dimension ref="A1:AD785"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -770,105 +768,105 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f>_xll.BDH(B$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
+        <f>_xll.BDH(B$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=783")</f>
         <v>43398</v>
       </c>
       <c r="B3" s="2">
         <v>1.44</v>
       </c>
       <c r="C3" s="1">
-        <f>_xll.BDH(D$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=747")</f>
+        <f>_xll.BDH(D$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=781")</f>
         <v>43398</v>
       </c>
       <c r="D3" s="2">
         <v>1.3774999999999999</v>
       </c>
       <c r="E3" s="1">
-        <f>_xll.BDH(F$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
+        <f>_xll.BDH(F$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=783")</f>
         <v>43398</v>
       </c>
       <c r="F3" s="2">
         <v>1.3674999999999999</v>
       </c>
       <c r="G3" s="1">
-        <f>_xll.BDH(H$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
+        <f>_xll.BDH(H$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=783")</f>
         <v>43398</v>
       </c>
       <c r="H3" s="2">
         <v>1.3774999999999999</v>
       </c>
       <c r="I3" s="1">
-        <f>_xll.BDH(J$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
+        <f>_xll.BDH(J$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=783")</f>
         <v>43398</v>
       </c>
       <c r="J3" s="2">
         <v>1.4</v>
       </c>
       <c r="K3" s="1">
-        <f>_xll.BDH(L$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
+        <f>_xll.BDH(L$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=783")</f>
         <v>43398</v>
       </c>
       <c r="L3" s="2">
         <v>1.4224999999999999</v>
       </c>
       <c r="M3" s="1">
-        <f>_xll.BDH(N$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
+        <f>_xll.BDH(N$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=783")</f>
         <v>43398</v>
       </c>
       <c r="N3" s="2">
         <v>1.4475</v>
       </c>
       <c r="O3" s="1">
-        <f>_xll.BDH(P$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
+        <f>_xll.BDH(P$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=783")</f>
         <v>43398</v>
       </c>
       <c r="P3" s="2">
         <v>1.4750000000000001</v>
       </c>
       <c r="Q3" s="1">
-        <f>_xll.BDH(R$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
+        <f>_xll.BDH(R$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=783")</f>
         <v>43398</v>
       </c>
       <c r="R3" s="2">
         <v>1.5024999999999999</v>
       </c>
       <c r="S3" s="1">
-        <f>_xll.BDH(T$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
+        <f>_xll.BDH(T$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=783")</f>
         <v>43398</v>
       </c>
       <c r="T3" s="2">
         <v>1.5325</v>
       </c>
       <c r="U3" s="1">
-        <f>_xll.BDH(V$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
+        <f>_xll.BDH(V$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=783")</f>
         <v>43398</v>
       </c>
       <c r="V3" s="2">
         <v>1.585</v>
       </c>
       <c r="W3" s="1">
-        <f>_xll.BDH(X$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
+        <f>_xll.BDH(X$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=783")</f>
         <v>43398</v>
       </c>
       <c r="X3" s="2">
         <v>1.67</v>
       </c>
       <c r="Y3" s="1">
-        <f>_xll.BDH(Z$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
+        <f>_xll.BDH(Z$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=783")</f>
         <v>43398</v>
       </c>
       <c r="Z3" s="2">
         <v>1.7850000000000001</v>
       </c>
       <c r="AA3" s="1">
-        <f>_xll.BDH(AB$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
+        <f>_xll.BDH(AB$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=783")</f>
         <v>43398</v>
       </c>
       <c r="AB3" s="2">
         <v>1.87</v>
       </c>
       <c r="AC3" s="1">
-        <f>_xll.BDH(AD$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=749")</f>
+        <f>_xll.BDH(AD$1, "PX_LAST", "1/1/1900", _xll.BToday(), "Dates", "S","cols=2;rows=783")</f>
         <v>43398</v>
       </c>
       <c r="AD3" s="2">
@@ -69426,7 +69424,7 @@
         <v>44446</v>
       </c>
       <c r="D749">
-        <v>1.925</v>
+        <v>1.9325000000000001</v>
       </c>
       <c r="E749" s="3">
         <v>44442</v>
@@ -69514,6 +69512,12 @@
       <c r="B750">
         <v>2.3875000000000002</v>
       </c>
+      <c r="C750" s="3">
+        <v>44447</v>
+      </c>
+      <c r="D750">
+        <v>1.9675</v>
+      </c>
       <c r="E750" s="3">
         <v>44445</v>
       </c>
@@ -69598,85 +69602,3207 @@
         <v>44446</v>
       </c>
       <c r="B751">
-        <v>2.37</v>
+        <v>2.3824999999999998</v>
+      </c>
+      <c r="C751" s="3">
+        <v>44448</v>
+      </c>
+      <c r="D751">
+        <v>1.9975000000000001</v>
       </c>
       <c r="E751" s="3">
         <v>44446</v>
       </c>
       <c r="F751">
-        <v>1.8149999999999999</v>
+        <v>1.8225</v>
       </c>
       <c r="G751" s="3">
         <v>44446</v>
       </c>
       <c r="H751">
-        <v>1.7925</v>
+        <v>1.7974999999999999</v>
       </c>
       <c r="I751" s="3">
         <v>44446</v>
       </c>
       <c r="J751">
-        <v>1.7774999999999999</v>
+        <v>1.7825</v>
       </c>
       <c r="K751" s="3">
         <v>44446</v>
       </c>
       <c r="L751">
-        <v>1.77</v>
+        <v>1.7749999999999999</v>
       </c>
       <c r="M751" s="3">
         <v>44446</v>
       </c>
       <c r="N751">
-        <v>1.7625</v>
+        <v>1.7675000000000001</v>
       </c>
       <c r="O751" s="3">
         <v>44446</v>
       </c>
       <c r="P751">
-        <v>1.7625</v>
+        <v>1.7675000000000001</v>
       </c>
       <c r="Q751" s="3">
         <v>44446</v>
       </c>
       <c r="R751">
-        <v>1.7574999999999998</v>
+        <v>1.7625</v>
       </c>
       <c r="S751" s="3">
         <v>44446</v>
       </c>
       <c r="T751">
-        <v>1.76</v>
+        <v>1.7650000000000001</v>
       </c>
       <c r="U751" s="3">
         <v>44446</v>
       </c>
       <c r="V751">
-        <v>1.7725</v>
+        <v>1.7774999999999999</v>
       </c>
       <c r="W751" s="3">
         <v>44446</v>
       </c>
       <c r="X751">
-        <v>1.825</v>
+        <v>1.8275000000000001</v>
       </c>
       <c r="Y751" s="3">
         <v>44446</v>
       </c>
       <c r="Z751">
-        <v>1.8774999999999999</v>
+        <v>1.88</v>
       </c>
       <c r="AA751" s="3">
         <v>44446</v>
       </c>
       <c r="AB751">
-        <v>1.915</v>
+        <v>1.9125000000000001</v>
       </c>
       <c r="AC751" s="3">
         <v>44446</v>
       </c>
       <c r="AD751">
+        <v>1.9375</v>
+      </c>
+    </row>
+    <row r="752" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A752" s="3">
+        <v>44447</v>
+      </c>
+      <c r="B752">
+        <v>2.42</v>
+      </c>
+      <c r="C752" s="3">
+        <v>44449</v>
+      </c>
+      <c r="D752">
+        <v>2.0674999999999999</v>
+      </c>
+      <c r="E752" s="3">
+        <v>44447</v>
+      </c>
+      <c r="F752">
+        <v>1.8525</v>
+      </c>
+      <c r="G752" s="3">
+        <v>44447</v>
+      </c>
+      <c r="H752">
+        <v>1.8225</v>
+      </c>
+      <c r="I752" s="3">
+        <v>44447</v>
+      </c>
+      <c r="J752">
+        <v>1.8075000000000001</v>
+      </c>
+      <c r="K752" s="3">
+        <v>44447</v>
+      </c>
+      <c r="L752">
+        <v>1.7974999999999999</v>
+      </c>
+      <c r="M752" s="3">
+        <v>44447</v>
+      </c>
+      <c r="N752">
+        <v>1.7875000000000001</v>
+      </c>
+      <c r="O752" s="3">
+        <v>44447</v>
+      </c>
+      <c r="P752">
+        <v>1.7850000000000001</v>
+      </c>
+      <c r="Q752" s="3">
+        <v>44447</v>
+      </c>
+      <c r="R752">
+        <v>1.78</v>
+      </c>
+      <c r="S752" s="3">
+        <v>44447</v>
+      </c>
+      <c r="T752">
+        <v>1.78</v>
+      </c>
+      <c r="U752" s="3">
+        <v>44447</v>
+      </c>
+      <c r="V752">
+        <v>1.7875000000000001</v>
+      </c>
+      <c r="W752" s="3">
+        <v>44447</v>
+      </c>
+      <c r="X752">
+        <v>1.835</v>
+      </c>
+      <c r="Y752" s="3">
+        <v>44447</v>
+      </c>
+      <c r="Z752">
+        <v>1.885</v>
+      </c>
+      <c r="AA752" s="3">
+        <v>44447</v>
+      </c>
+      <c r="AB752">
+        <v>1.9175</v>
+      </c>
+      <c r="AC752" s="3">
+        <v>44447</v>
+      </c>
+      <c r="AD752">
+        <v>1.9424999999999999</v>
+      </c>
+    </row>
+    <row r="753" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A753" s="3">
+        <v>44448</v>
+      </c>
+      <c r="B753">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="C753" s="3">
+        <v>44452</v>
+      </c>
+      <c r="D753">
+        <v>2.125</v>
+      </c>
+      <c r="E753" s="3">
+        <v>44448</v>
+      </c>
+      <c r="F753">
+        <v>1.8774999999999999</v>
+      </c>
+      <c r="G753" s="3">
+        <v>44448</v>
+      </c>
+      <c r="H753">
+        <v>1.8399999999999999</v>
+      </c>
+      <c r="I753" s="3">
+        <v>44448</v>
+      </c>
+      <c r="J753">
+        <v>1.8199999999999998</v>
+      </c>
+      <c r="K753" s="3">
+        <v>44448</v>
+      </c>
+      <c r="L753">
+        <v>1.8075000000000001</v>
+      </c>
+      <c r="M753" s="3">
+        <v>44448</v>
+      </c>
+      <c r="N753">
+        <v>1.7949999999999999</v>
+      </c>
+      <c r="O753" s="3">
+        <v>44448</v>
+      </c>
+      <c r="P753">
+        <v>1.79</v>
+      </c>
+      <c r="Q753" s="3">
+        <v>44448</v>
+      </c>
+      <c r="R753">
+        <v>1.7825</v>
+      </c>
+      <c r="S753" s="3">
+        <v>44448</v>
+      </c>
+      <c r="T753">
+        <v>1.7825</v>
+      </c>
+      <c r="U753" s="3">
+        <v>44448</v>
+      </c>
+      <c r="V753">
+        <v>1.7925</v>
+      </c>
+      <c r="W753" s="3">
+        <v>44448</v>
+      </c>
+      <c r="X753">
+        <v>1.8425</v>
+      </c>
+      <c r="Y753" s="3">
+        <v>44448</v>
+      </c>
+      <c r="Z753">
+        <v>1.8925000000000001</v>
+      </c>
+      <c r="AA753" s="3">
+        <v>44448</v>
+      </c>
+      <c r="AB753">
+        <v>1.9224999999999999</v>
+      </c>
+      <c r="AC753" s="3">
+        <v>44448</v>
+      </c>
+      <c r="AD753">
+        <v>1.9449999999999998</v>
+      </c>
+    </row>
+    <row r="754" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A754" s="3">
+        <v>44449</v>
+      </c>
+      <c r="B754">
+        <v>2.5274999999999999</v>
+      </c>
+      <c r="C754" s="3">
+        <v>44453</v>
+      </c>
+      <c r="D754">
+        <v>2.09</v>
+      </c>
+      <c r="E754" s="3">
+        <v>44449</v>
+      </c>
+      <c r="F754">
+        <v>1.9375</v>
+      </c>
+      <c r="G754" s="3">
+        <v>44449</v>
+      </c>
+      <c r="H754">
+        <v>1.885</v>
+      </c>
+      <c r="I754" s="3">
+        <v>44449</v>
+      </c>
+      <c r="J754">
+        <v>1.8525</v>
+      </c>
+      <c r="K754" s="3">
+        <v>44449</v>
+      </c>
+      <c r="L754">
+        <v>1.8399999999999999</v>
+      </c>
+      <c r="M754" s="3">
+        <v>44449</v>
+      </c>
+      <c r="N754">
+        <v>1.8275000000000001</v>
+      </c>
+      <c r="O754" s="3">
+        <v>44449</v>
+      </c>
+      <c r="P754">
+        <v>1.8225</v>
+      </c>
+      <c r="Q754" s="3">
+        <v>44449</v>
+      </c>
+      <c r="R754">
+        <v>1.8149999999999999</v>
+      </c>
+      <c r="S754" s="3">
+        <v>44449</v>
+      </c>
+      <c r="T754">
+        <v>1.8125</v>
+      </c>
+      <c r="U754" s="3">
+        <v>44449</v>
+      </c>
+      <c r="V754">
+        <v>1.8199999999999998</v>
+      </c>
+      <c r="W754" s="3">
+        <v>44449</v>
+      </c>
+      <c r="X754">
+        <v>1.865</v>
+      </c>
+      <c r="Y754" s="3">
+        <v>44449</v>
+      </c>
+      <c r="Z754">
+        <v>1.9125000000000001</v>
+      </c>
+      <c r="AA754" s="3">
+        <v>44449</v>
+      </c>
+      <c r="AB754">
+        <v>1.9424999999999999</v>
+      </c>
+      <c r="AC754" s="3">
+        <v>44449</v>
+      </c>
+      <c r="AD754">
+        <v>1.9624999999999999</v>
+      </c>
+    </row>
+    <row r="755" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A755" s="3">
+        <v>44452</v>
+      </c>
+      <c r="B755">
+        <v>2.59</v>
+      </c>
+      <c r="C755" s="3">
+        <v>44454</v>
+      </c>
+      <c r="D755">
+        <v>2.14</v>
+      </c>
+      <c r="E755" s="3">
+        <v>44452</v>
+      </c>
+      <c r="F755">
+        <v>1.9875</v>
+      </c>
+      <c r="G755" s="3">
+        <v>44452</v>
+      </c>
+      <c r="H755">
+        <v>1.9300000000000002</v>
+      </c>
+      <c r="I755" s="3">
+        <v>44452</v>
+      </c>
+      <c r="J755">
+        <v>1.895</v>
+      </c>
+      <c r="K755" s="3">
+        <v>44452</v>
+      </c>
+      <c r="L755">
+        <v>1.88</v>
+      </c>
+      <c r="M755" s="3">
+        <v>44452</v>
+      </c>
+      <c r="N755">
+        <v>1.8625</v>
+      </c>
+      <c r="O755" s="3">
+        <v>44452</v>
+      </c>
+      <c r="P755">
+        <v>1.855</v>
+      </c>
+      <c r="Q755" s="3">
+        <v>44452</v>
+      </c>
+      <c r="R755">
+        <v>1.845</v>
+      </c>
+      <c r="S755" s="3">
+        <v>44452</v>
+      </c>
+      <c r="T755">
+        <v>1.8399999999999999</v>
+      </c>
+      <c r="U755" s="3">
+        <v>44452</v>
+      </c>
+      <c r="V755">
+        <v>1.845</v>
+      </c>
+      <c r="W755" s="3">
+        <v>44452</v>
+      </c>
+      <c r="X755">
+        <v>1.8875</v>
+      </c>
+      <c r="Y755" s="3">
+        <v>44452</v>
+      </c>
+      <c r="Z755">
+        <v>1.9300000000000002</v>
+      </c>
+      <c r="AA755" s="3">
+        <v>44452</v>
+      </c>
+      <c r="AB755">
+        <v>1.9550000000000001</v>
+      </c>
+      <c r="AC755" s="3">
+        <v>44452</v>
+      </c>
+      <c r="AD755">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="756" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A756" s="3">
+        <v>44453</v>
+      </c>
+      <c r="B756">
+        <v>2.5674999999999999</v>
+      </c>
+      <c r="C756" s="3">
+        <v>44455</v>
+      </c>
+      <c r="D756">
+        <v>2.1274999999999999</v>
+      </c>
+      <c r="E756" s="3">
+        <v>44453</v>
+      </c>
+      <c r="F756">
+        <v>1.95</v>
+      </c>
+      <c r="G756" s="3">
+        <v>44453</v>
+      </c>
+      <c r="H756">
+        <v>1.8875</v>
+      </c>
+      <c r="I756" s="3">
+        <v>44453</v>
+      </c>
+      <c r="J756">
+        <v>1.85</v>
+      </c>
+      <c r="K756" s="3">
+        <v>44453</v>
+      </c>
+      <c r="L756">
+        <v>1.835</v>
+      </c>
+      <c r="M756" s="3">
+        <v>44453</v>
+      </c>
+      <c r="N756">
+        <v>1.8174999999999999</v>
+      </c>
+      <c r="O756" s="3">
+        <v>44453</v>
+      </c>
+      <c r="P756">
+        <v>1.81</v>
+      </c>
+      <c r="Q756" s="3">
+        <v>44453</v>
+      </c>
+      <c r="R756">
+        <v>1.8</v>
+      </c>
+      <c r="S756" s="3">
+        <v>44453</v>
+      </c>
+      <c r="T756">
+        <v>1.7949999999999999</v>
+      </c>
+      <c r="U756" s="3">
+        <v>44453</v>
+      </c>
+      <c r="V756">
+        <v>1.8050000000000002</v>
+      </c>
+      <c r="W756" s="3">
+        <v>44453</v>
+      </c>
+      <c r="X756">
+        <v>1.8475000000000001</v>
+      </c>
+      <c r="Y756" s="3">
+        <v>44453</v>
+      </c>
+      <c r="Z756">
+        <v>1.8900000000000001</v>
+      </c>
+      <c r="AA756" s="3">
+        <v>44453</v>
+      </c>
+      <c r="AB756">
+        <v>1.915</v>
+      </c>
+      <c r="AC756" s="3">
+        <v>44453</v>
+      </c>
+      <c r="AD756">
+        <v>1.9300000000000002</v>
+      </c>
+    </row>
+    <row r="757" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A757" s="3">
+        <v>44454</v>
+      </c>
+      <c r="B757">
+        <v>2.625</v>
+      </c>
+      <c r="C757" s="3">
+        <v>44456</v>
+      </c>
+      <c r="D757">
+        <v>2.1074999999999999</v>
+      </c>
+      <c r="E757" s="3">
+        <v>44454</v>
+      </c>
+      <c r="F757">
+        <v>1.9875</v>
+      </c>
+      <c r="G757" s="3">
+        <v>44454</v>
+      </c>
+      <c r="H757">
+        <v>1.9175</v>
+      </c>
+      <c r="I757" s="3">
+        <v>44454</v>
+      </c>
+      <c r="J757">
+        <v>1.875</v>
+      </c>
+      <c r="K757" s="3">
+        <v>44454</v>
+      </c>
+      <c r="L757">
+        <v>1.8574999999999999</v>
+      </c>
+      <c r="M757" s="3">
+        <v>44454</v>
+      </c>
+      <c r="N757">
+        <v>1.8325</v>
+      </c>
+      <c r="O757" s="3">
+        <v>44454</v>
+      </c>
+      <c r="P757">
+        <v>1.8225</v>
+      </c>
+      <c r="Q757" s="3">
+        <v>44454</v>
+      </c>
+      <c r="R757">
+        <v>1.8075000000000001</v>
+      </c>
+      <c r="S757" s="3">
+        <v>44454</v>
+      </c>
+      <c r="T757">
+        <v>1.8</v>
+      </c>
+      <c r="U757" s="3">
+        <v>44454</v>
+      </c>
+      <c r="V757">
+        <v>1.8050000000000002</v>
+      </c>
+      <c r="W757" s="3">
+        <v>44454</v>
+      </c>
+      <c r="X757">
+        <v>1.845</v>
+      </c>
+      <c r="Y757" s="3">
+        <v>44454</v>
+      </c>
+      <c r="Z757">
+        <v>1.8925000000000001</v>
+      </c>
+      <c r="AA757" s="3">
+        <v>44454</v>
+      </c>
+      <c r="AB757">
+        <v>1.92</v>
+      </c>
+      <c r="AC757" s="3">
+        <v>44454</v>
+      </c>
+      <c r="AD757">
+        <v>1.9375</v>
+      </c>
+    </row>
+    <row r="758" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A758" s="3">
+        <v>44455</v>
+      </c>
+      <c r="B758">
+        <v>2.61</v>
+      </c>
+      <c r="C758" s="3">
+        <v>44459</v>
+      </c>
+      <c r="D758">
+        <v>2.0625</v>
+      </c>
+      <c r="E758" s="3">
+        <v>44455</v>
+      </c>
+      <c r="F758">
+        <v>1.9750000000000001</v>
+      </c>
+      <c r="G758" s="3">
+        <v>44455</v>
+      </c>
+      <c r="H758">
+        <v>1.9075</v>
+      </c>
+      <c r="I758" s="3">
+        <v>44455</v>
+      </c>
+      <c r="J758">
+        <v>1.865</v>
+      </c>
+      <c r="K758" s="3">
+        <v>44455</v>
+      </c>
+      <c r="L758">
+        <v>1.8425</v>
+      </c>
+      <c r="M758" s="3">
+        <v>44455</v>
+      </c>
+      <c r="N758">
+        <v>1.825</v>
+      </c>
+      <c r="O758" s="3">
+        <v>44455</v>
+      </c>
+      <c r="P758">
+        <v>1.8149999999999999</v>
+      </c>
+      <c r="Q758" s="3">
+        <v>44455</v>
+      </c>
+      <c r="R758">
+        <v>1.8050000000000002</v>
+      </c>
+      <c r="S758" s="3">
+        <v>44455</v>
+      </c>
+      <c r="T758">
+        <v>1.8</v>
+      </c>
+      <c r="U758" s="3">
+        <v>44455</v>
+      </c>
+      <c r="V758">
+        <v>1.8050000000000002</v>
+      </c>
+      <c r="W758" s="3">
+        <v>44455</v>
+      </c>
+      <c r="X758">
+        <v>1.845</v>
+      </c>
+      <c r="Y758" s="3">
+        <v>44455</v>
+      </c>
+      <c r="Z758">
+        <v>1.8925000000000001</v>
+      </c>
+      <c r="AA758" s="3">
+        <v>44455</v>
+      </c>
+      <c r="AB758">
+        <v>1.9224999999999999</v>
+      </c>
+      <c r="AC758" s="3">
+        <v>44455</v>
+      </c>
+      <c r="AD758">
+        <v>1.9424999999999999</v>
+      </c>
+    </row>
+    <row r="759" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A759" s="3">
+        <v>44456</v>
+      </c>
+      <c r="B759">
+        <v>2.59</v>
+      </c>
+      <c r="C759" s="3">
+        <v>44460</v>
+      </c>
+      <c r="D759">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="E759" s="3">
+        <v>44456</v>
+      </c>
+      <c r="F759">
+        <v>1.9649999999999999</v>
+      </c>
+      <c r="G759" s="3">
+        <v>44456</v>
+      </c>
+      <c r="H759">
+        <v>1.905</v>
+      </c>
+      <c r="I759" s="3">
+        <v>44456</v>
+      </c>
+      <c r="J759">
+        <v>1.87</v>
+      </c>
+      <c r="K759" s="3">
+        <v>44456</v>
+      </c>
+      <c r="L759">
+        <v>1.8475000000000001</v>
+      </c>
+      <c r="M759" s="3">
+        <v>44456</v>
+      </c>
+      <c r="N759">
+        <v>1.83</v>
+      </c>
+      <c r="O759" s="3">
+        <v>44456</v>
+      </c>
+      <c r="P759">
+        <v>1.8225</v>
+      </c>
+      <c r="Q759" s="3">
+        <v>44456</v>
+      </c>
+      <c r="R759">
+        <v>1.8125</v>
+      </c>
+      <c r="S759" s="3">
+        <v>44456</v>
+      </c>
+      <c r="T759">
+        <v>1.8075000000000001</v>
+      </c>
+      <c r="U759" s="3">
+        <v>44456</v>
+      </c>
+      <c r="V759">
+        <v>1.8149999999999999</v>
+      </c>
+      <c r="W759" s="3">
+        <v>44456</v>
+      </c>
+      <c r="X759">
+        <v>1.8574999999999999</v>
+      </c>
+      <c r="Y759" s="3">
+        <v>44456</v>
+      </c>
+      <c r="Z759">
+        <v>1.905</v>
+      </c>
+      <c r="AA759" s="3">
+        <v>44456</v>
+      </c>
+      <c r="AB759">
+        <v>1.9350000000000001</v>
+      </c>
+      <c r="AC759" s="3">
+        <v>44456</v>
+      </c>
+      <c r="AD759">
+        <v>1.9550000000000001</v>
+      </c>
+    </row>
+    <row r="760" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A760" s="3">
+        <v>44459</v>
+      </c>
+      <c r="B760">
+        <v>2.5449999999999999</v>
+      </c>
+      <c r="C760" s="3">
+        <v>44461</v>
+      </c>
+      <c r="D760">
+        <v>2.09</v>
+      </c>
+      <c r="E760" s="3">
+        <v>44459</v>
+      </c>
+      <c r="F760">
+        <v>1.92</v>
+      </c>
+      <c r="G760" s="3">
+        <v>44459</v>
+      </c>
+      <c r="H760">
+        <v>1.8625</v>
+      </c>
+      <c r="I760" s="3">
+        <v>44459</v>
+      </c>
+      <c r="J760">
+        <v>1.8275000000000001</v>
+      </c>
+      <c r="K760" s="3">
+        <v>44459</v>
+      </c>
+      <c r="L760">
+        <v>1.8050000000000002</v>
+      </c>
+      <c r="M760" s="3">
+        <v>44459</v>
+      </c>
+      <c r="N760">
+        <v>1.79</v>
+      </c>
+      <c r="O760" s="3">
+        <v>44459</v>
+      </c>
+      <c r="P760">
+        <v>1.7825</v>
+      </c>
+      <c r="Q760" s="3">
+        <v>44459</v>
+      </c>
+      <c r="R760">
+        <v>1.7749999999999999</v>
+      </c>
+      <c r="S760" s="3">
+        <v>44459</v>
+      </c>
+      <c r="T760">
+        <v>1.7725</v>
+      </c>
+      <c r="U760" s="3">
+        <v>44459</v>
+      </c>
+      <c r="V760">
+        <v>1.78</v>
+      </c>
+      <c r="W760" s="3">
+        <v>44459</v>
+      </c>
+      <c r="X760">
+        <v>1.825</v>
+      </c>
+      <c r="Y760" s="3">
+        <v>44459</v>
+      </c>
+      <c r="Z760">
+        <v>1.8774999999999999</v>
+      </c>
+      <c r="AA760" s="3">
+        <v>44459</v>
+      </c>
+      <c r="AB760">
+        <v>1.9075</v>
+      </c>
+      <c r="AC760" s="3">
+        <v>44459</v>
+      </c>
+      <c r="AD760">
+        <v>1.9275</v>
+      </c>
+    </row>
+    <row r="761" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A761" s="3">
+        <v>44460</v>
+      </c>
+      <c r="B761">
+        <v>2.54</v>
+      </c>
+      <c r="C761" s="3">
+        <v>44462</v>
+      </c>
+      <c r="D761">
+        <v>2.125</v>
+      </c>
+      <c r="E761" s="3">
+        <v>44460</v>
+      </c>
+      <c r="F761">
+        <v>1.925</v>
+      </c>
+      <c r="G761" s="3">
+        <v>44460</v>
+      </c>
+      <c r="H761">
+        <v>1.8675000000000002</v>
+      </c>
+      <c r="I761" s="3">
+        <v>44460</v>
+      </c>
+      <c r="J761">
+        <v>1.835</v>
+      </c>
+      <c r="K761" s="3">
+        <v>44460</v>
+      </c>
+      <c r="L761">
+        <v>1.8125</v>
+      </c>
+      <c r="M761" s="3">
+        <v>44460</v>
+      </c>
+      <c r="N761">
+        <v>1.7974999999999999</v>
+      </c>
+      <c r="O761" s="3">
+        <v>44460</v>
+      </c>
+      <c r="P761">
+        <v>1.79</v>
+      </c>
+      <c r="Q761" s="3">
+        <v>44460</v>
+      </c>
+      <c r="R761">
+        <v>1.7850000000000001</v>
+      </c>
+      <c r="S761" s="3">
+        <v>44460</v>
+      </c>
+      <c r="T761">
+        <v>1.7825</v>
+      </c>
+      <c r="U761" s="3">
+        <v>44460</v>
+      </c>
+      <c r="V761">
+        <v>1.79</v>
+      </c>
+      <c r="W761" s="3">
+        <v>44460</v>
+      </c>
+      <c r="X761">
+        <v>1.835</v>
+      </c>
+      <c r="Y761" s="3">
+        <v>44460</v>
+      </c>
+      <c r="Z761">
+        <v>1.8875</v>
+      </c>
+      <c r="AA761" s="3">
+        <v>44460</v>
+      </c>
+      <c r="AB761">
+        <v>1.9175</v>
+      </c>
+      <c r="AC761" s="3">
+        <v>44460</v>
+      </c>
+      <c r="AD761">
         <v>1.94</v>
+      </c>
+    </row>
+    <row r="762" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A762" s="3">
+        <v>44461</v>
+      </c>
+      <c r="B762">
+        <v>2.5750000000000002</v>
+      </c>
+      <c r="C762" s="3">
+        <v>44463</v>
+      </c>
+      <c r="D762">
+        <v>2.1025</v>
+      </c>
+      <c r="E762" s="3">
+        <v>44461</v>
+      </c>
+      <c r="F762">
+        <v>1.9350000000000001</v>
+      </c>
+      <c r="G762" s="3">
+        <v>44461</v>
+      </c>
+      <c r="H762">
+        <v>1.87</v>
+      </c>
+      <c r="I762" s="3">
+        <v>44461</v>
+      </c>
+      <c r="J762">
+        <v>1.835</v>
+      </c>
+      <c r="K762" s="3">
+        <v>44461</v>
+      </c>
+      <c r="L762">
+        <v>1.8149999999999999</v>
+      </c>
+      <c r="M762" s="3">
+        <v>44461</v>
+      </c>
+      <c r="N762">
+        <v>1.7974999999999999</v>
+      </c>
+      <c r="O762" s="3">
+        <v>44461</v>
+      </c>
+      <c r="P762">
+        <v>1.7925</v>
+      </c>
+      <c r="Q762" s="3">
+        <v>44461</v>
+      </c>
+      <c r="R762">
+        <v>1.7875000000000001</v>
+      </c>
+      <c r="S762" s="3">
+        <v>44461</v>
+      </c>
+      <c r="T762">
+        <v>1.7850000000000001</v>
+      </c>
+      <c r="U762" s="3">
+        <v>44461</v>
+      </c>
+      <c r="V762">
+        <v>1.7925</v>
+      </c>
+      <c r="W762" s="3">
+        <v>44461</v>
+      </c>
+      <c r="X762">
+        <v>1.8399999999999999</v>
+      </c>
+      <c r="Y762" s="3">
+        <v>44461</v>
+      </c>
+      <c r="Z762">
+        <v>1.8900000000000001</v>
+      </c>
+      <c r="AA762" s="3">
+        <v>44461</v>
+      </c>
+      <c r="AB762">
+        <v>1.9224999999999999</v>
+      </c>
+      <c r="AC762" s="3">
+        <v>44461</v>
+      </c>
+      <c r="AD762">
+        <v>1.9449999999999998</v>
+      </c>
+    </row>
+    <row r="763" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A763" s="3">
+        <v>44462</v>
+      </c>
+      <c r="B763">
+        <v>2.6074999999999999</v>
+      </c>
+      <c r="C763" s="3">
+        <v>44466</v>
+      </c>
+      <c r="D763">
+        <v>2.1775000000000002</v>
+      </c>
+      <c r="E763" s="3">
+        <v>44462</v>
+      </c>
+      <c r="F763">
+        <v>1.9624999999999999</v>
+      </c>
+      <c r="G763" s="3">
+        <v>44462</v>
+      </c>
+      <c r="H763">
+        <v>1.8900000000000001</v>
+      </c>
+      <c r="I763" s="3">
+        <v>44462</v>
+      </c>
+      <c r="J763">
+        <v>1.85</v>
+      </c>
+      <c r="K763" s="3">
+        <v>44462</v>
+      </c>
+      <c r="L763">
+        <v>1.8275000000000001</v>
+      </c>
+      <c r="M763" s="3">
+        <v>44462</v>
+      </c>
+      <c r="N763">
+        <v>1.8125</v>
+      </c>
+      <c r="O763" s="3">
+        <v>44462</v>
+      </c>
+      <c r="P763">
+        <v>1.8075000000000001</v>
+      </c>
+      <c r="Q763" s="3">
+        <v>44462</v>
+      </c>
+      <c r="R763">
+        <v>1.8050000000000002</v>
+      </c>
+      <c r="S763" s="3">
+        <v>44462</v>
+      </c>
+      <c r="T763">
+        <v>1.8025</v>
+      </c>
+      <c r="U763" s="3">
+        <v>44462</v>
+      </c>
+      <c r="V763">
+        <v>1.8125</v>
+      </c>
+      <c r="W763" s="3">
+        <v>44462</v>
+      </c>
+      <c r="X763">
+        <v>1.8625</v>
+      </c>
+      <c r="Y763" s="3">
+        <v>44462</v>
+      </c>
+      <c r="Z763">
+        <v>1.915</v>
+      </c>
+      <c r="AA763" s="3">
+        <v>44462</v>
+      </c>
+      <c r="AB763">
+        <v>1.9449999999999998</v>
+      </c>
+      <c r="AC763" s="3">
+        <v>44462</v>
+      </c>
+      <c r="AD763">
+        <v>1.9675</v>
+      </c>
+    </row>
+    <row r="764" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A764" s="3">
+        <v>44463</v>
+      </c>
+      <c r="B764">
+        <v>2.5949999999999998</v>
+      </c>
+      <c r="C764" s="3">
+        <v>44467</v>
+      </c>
+      <c r="D764">
+        <v>2.2574999999999998</v>
+      </c>
+      <c r="E764" s="3">
+        <v>44463</v>
+      </c>
+      <c r="F764">
+        <v>1.9325000000000001</v>
+      </c>
+      <c r="G764" s="3">
+        <v>44463</v>
+      </c>
+      <c r="H764">
+        <v>1.865</v>
+      </c>
+      <c r="I764" s="3">
+        <v>44463</v>
+      </c>
+      <c r="J764">
+        <v>1.83</v>
+      </c>
+      <c r="K764" s="3">
+        <v>44463</v>
+      </c>
+      <c r="L764">
+        <v>1.81</v>
+      </c>
+      <c r="M764" s="3">
+        <v>44463</v>
+      </c>
+      <c r="N764">
+        <v>1.7949999999999999</v>
+      </c>
+      <c r="O764" s="3">
+        <v>44463</v>
+      </c>
+      <c r="P764">
+        <v>1.7925</v>
+      </c>
+      <c r="Q764" s="3">
+        <v>44463</v>
+      </c>
+      <c r="R764">
+        <v>1.79</v>
+      </c>
+      <c r="S764" s="3">
+        <v>44463</v>
+      </c>
+      <c r="T764">
+        <v>1.7875000000000001</v>
+      </c>
+      <c r="U764" s="3">
+        <v>44463</v>
+      </c>
+      <c r="V764">
+        <v>1.8</v>
+      </c>
+      <c r="W764" s="3">
+        <v>44463</v>
+      </c>
+      <c r="X764">
+        <v>1.85</v>
+      </c>
+      <c r="Y764" s="3">
+        <v>44463</v>
+      </c>
+      <c r="Z764">
+        <v>1.9024999999999999</v>
+      </c>
+      <c r="AA764" s="3">
+        <v>44463</v>
+      </c>
+      <c r="AB764">
+        <v>1.9325000000000001</v>
+      </c>
+      <c r="AC764" s="3">
+        <v>44463</v>
+      </c>
+      <c r="AD764">
+        <v>1.9575</v>
+      </c>
+    </row>
+    <row r="765" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A765" s="3">
+        <v>44466</v>
+      </c>
+      <c r="B765">
+        <v>2.6724999999999999</v>
+      </c>
+      <c r="C765" s="3">
+        <v>44468</v>
+      </c>
+      <c r="D765">
+        <v>2.2725</v>
+      </c>
+      <c r="E765" s="3">
+        <v>44466</v>
+      </c>
+      <c r="F765">
+        <v>2</v>
+      </c>
+      <c r="G765" s="3">
+        <v>44466</v>
+      </c>
+      <c r="H765">
+        <v>1.925</v>
+      </c>
+      <c r="I765" s="3">
+        <v>44466</v>
+      </c>
+      <c r="J765">
+        <v>1.885</v>
+      </c>
+      <c r="K765" s="3">
+        <v>44466</v>
+      </c>
+      <c r="L765">
+        <v>1.8599999999999999</v>
+      </c>
+      <c r="M765" s="3">
+        <v>44466</v>
+      </c>
+      <c r="N765">
+        <v>1.845</v>
+      </c>
+      <c r="O765" s="3">
+        <v>44466</v>
+      </c>
+      <c r="P765">
+        <v>1.8374999999999999</v>
+      </c>
+      <c r="Q765" s="3">
+        <v>44466</v>
+      </c>
+      <c r="R765">
+        <v>1.8325</v>
+      </c>
+      <c r="S765" s="3">
+        <v>44466</v>
+      </c>
+      <c r="T765">
+        <v>1.835</v>
+      </c>
+      <c r="U765" s="3">
+        <v>44466</v>
+      </c>
+      <c r="V765">
+        <v>1.85</v>
+      </c>
+      <c r="W765" s="3">
+        <v>44466</v>
+      </c>
+      <c r="X765">
+        <v>1.8975</v>
+      </c>
+      <c r="Y765" s="3">
+        <v>44466</v>
+      </c>
+      <c r="Z765">
+        <v>1.9475</v>
+      </c>
+      <c r="AA765" s="3">
+        <v>44466</v>
+      </c>
+      <c r="AB765">
+        <v>1.9775</v>
+      </c>
+      <c r="AC765" s="3">
+        <v>44466</v>
+      </c>
+      <c r="AD765">
+        <v>1.9975000000000001</v>
+      </c>
+    </row>
+    <row r="766" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A766" s="3">
+        <v>44467</v>
+      </c>
+      <c r="B766">
+        <v>2.77</v>
+      </c>
+      <c r="C766" s="3">
+        <v>44469</v>
+      </c>
+      <c r="D766">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E766" s="3">
+        <v>44467</v>
+      </c>
+      <c r="F766">
+        <v>2.0649999999999999</v>
+      </c>
+      <c r="G766" s="3">
+        <v>44467</v>
+      </c>
+      <c r="H766">
+        <v>1.9849999999999999</v>
+      </c>
+      <c r="I766" s="3">
+        <v>44467</v>
+      </c>
+      <c r="J766">
+        <v>1.9375</v>
+      </c>
+      <c r="K766" s="3">
+        <v>44467</v>
+      </c>
+      <c r="L766">
+        <v>1.9075</v>
+      </c>
+      <c r="M766" s="3">
+        <v>44467</v>
+      </c>
+      <c r="N766">
+        <v>1.885</v>
+      </c>
+      <c r="O766" s="3">
+        <v>44467</v>
+      </c>
+      <c r="P766">
+        <v>1.875</v>
+      </c>
+      <c r="Q766" s="3">
+        <v>44467</v>
+      </c>
+      <c r="R766">
+        <v>1.8625</v>
+      </c>
+      <c r="S766" s="3">
+        <v>44467</v>
+      </c>
+      <c r="T766">
+        <v>1.8625</v>
+      </c>
+      <c r="U766" s="3">
+        <v>44467</v>
+      </c>
+      <c r="V766">
+        <v>1.8725000000000001</v>
+      </c>
+      <c r="W766" s="3">
+        <v>44467</v>
+      </c>
+      <c r="X766">
+        <v>1.915</v>
+      </c>
+      <c r="Y766" s="3">
+        <v>44467</v>
+      </c>
+      <c r="Z766">
+        <v>1.96</v>
+      </c>
+      <c r="AA766" s="3">
+        <v>44467</v>
+      </c>
+      <c r="AB766">
+        <v>1.9875</v>
+      </c>
+      <c r="AC766" s="3">
+        <v>44467</v>
+      </c>
+      <c r="AD766">
+        <v>2.0074999999999998</v>
+      </c>
+    </row>
+    <row r="767" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A767" s="3">
+        <v>44468</v>
+      </c>
+      <c r="B767">
+        <v>2.8</v>
+      </c>
+      <c r="C767" s="3">
+        <v>44470</v>
+      </c>
+      <c r="D767">
+        <v>2.17</v>
+      </c>
+      <c r="E767" s="3">
+        <v>44468</v>
+      </c>
+      <c r="F767">
+        <v>2.0724999999999998</v>
+      </c>
+      <c r="G767" s="3">
+        <v>44468</v>
+      </c>
+      <c r="H767">
+        <v>1.9750000000000001</v>
+      </c>
+      <c r="I767" s="3">
+        <v>44468</v>
+      </c>
+      <c r="J767">
+        <v>1.92</v>
+      </c>
+      <c r="K767" s="3">
+        <v>44468</v>
+      </c>
+      <c r="L767">
+        <v>1.8900000000000001</v>
+      </c>
+      <c r="M767" s="3">
+        <v>44468</v>
+      </c>
+      <c r="N767">
+        <v>1.8675000000000002</v>
+      </c>
+      <c r="O767" s="3">
+        <v>44468</v>
+      </c>
+      <c r="P767">
+        <v>1.8574999999999999</v>
+      </c>
+      <c r="Q767" s="3">
+        <v>44468</v>
+      </c>
+      <c r="R767">
+        <v>1.8475000000000001</v>
+      </c>
+      <c r="S767" s="3">
+        <v>44468</v>
+      </c>
+      <c r="T767">
+        <v>1.8475000000000001</v>
+      </c>
+      <c r="U767" s="3">
+        <v>44468</v>
+      </c>
+      <c r="V767">
+        <v>1.8599999999999999</v>
+      </c>
+      <c r="W767" s="3">
+        <v>44468</v>
+      </c>
+      <c r="X767">
+        <v>1.905</v>
+      </c>
+      <c r="Y767" s="3">
+        <v>44468</v>
+      </c>
+      <c r="Z767">
+        <v>1.9525000000000001</v>
+      </c>
+      <c r="AA767" s="3">
+        <v>44468</v>
+      </c>
+      <c r="AB767">
+        <v>1.9824999999999999</v>
+      </c>
+      <c r="AC767" s="3">
+        <v>44468</v>
+      </c>
+      <c r="AD767">
+        <v>2.0074999999999998</v>
+      </c>
+    </row>
+    <row r="768" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A768" s="3">
+        <v>44469</v>
+      </c>
+      <c r="B768">
+        <v>2.8449999999999998</v>
+      </c>
+      <c r="C768" s="3">
+        <v>44473</v>
+      </c>
+      <c r="D768">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E768" s="3">
+        <v>44469</v>
+      </c>
+      <c r="F768">
+        <v>2.09</v>
+      </c>
+      <c r="G768" s="3">
+        <v>44469</v>
+      </c>
+      <c r="H768">
+        <v>1.9824999999999999</v>
+      </c>
+      <c r="I768" s="3">
+        <v>44469</v>
+      </c>
+      <c r="J768">
+        <v>1.925</v>
+      </c>
+      <c r="K768" s="3">
+        <v>44469</v>
+      </c>
+      <c r="L768">
+        <v>1.8925000000000001</v>
+      </c>
+      <c r="M768" s="3">
+        <v>44469</v>
+      </c>
+      <c r="N768">
+        <v>1.87</v>
+      </c>
+      <c r="O768" s="3">
+        <v>44469</v>
+      </c>
+      <c r="P768">
+        <v>1.8574999999999999</v>
+      </c>
+      <c r="Q768" s="3">
+        <v>44469</v>
+      </c>
+      <c r="R768">
+        <v>1.8475000000000001</v>
+      </c>
+      <c r="S768" s="3">
+        <v>44469</v>
+      </c>
+      <c r="T768">
+        <v>1.85</v>
+      </c>
+      <c r="U768" s="3">
+        <v>44469</v>
+      </c>
+      <c r="V768">
+        <v>1.865</v>
+      </c>
+      <c r="W768" s="3">
+        <v>44469</v>
+      </c>
+      <c r="X768">
+        <v>1.9100000000000001</v>
+      </c>
+      <c r="Y768" s="3">
+        <v>44469</v>
+      </c>
+      <c r="Z768">
+        <v>1.9575</v>
+      </c>
+      <c r="AA768" s="3">
+        <v>44469</v>
+      </c>
+      <c r="AB768">
+        <v>1.99</v>
+      </c>
+      <c r="AC768" s="3">
+        <v>44469</v>
+      </c>
+      <c r="AD768">
+        <v>2.0150000000000001</v>
+      </c>
+    </row>
+    <row r="769" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A769" s="3">
+        <v>44470</v>
+      </c>
+      <c r="B769">
+        <v>2.4925000000000002</v>
+      </c>
+      <c r="C769" s="3">
+        <v>44474</v>
+      </c>
+      <c r="D769">
+        <v>2.3675000000000002</v>
+      </c>
+      <c r="E769" s="3">
+        <v>44470</v>
+      </c>
+      <c r="F769">
+        <v>2.0249999999999999</v>
+      </c>
+      <c r="G769" s="3">
+        <v>44470</v>
+      </c>
+      <c r="H769">
+        <v>1.9449999999999998</v>
+      </c>
+      <c r="I769" s="3">
+        <v>44470</v>
+      </c>
+      <c r="J769">
+        <v>1.905</v>
+      </c>
+      <c r="K769" s="3">
+        <v>44470</v>
+      </c>
+      <c r="L769">
+        <v>1.8824999999999998</v>
+      </c>
+      <c r="M769" s="3">
+        <v>44470</v>
+      </c>
+      <c r="N769">
+        <v>1.8625</v>
+      </c>
+      <c r="O769" s="3">
+        <v>44470</v>
+      </c>
+      <c r="P769">
+        <v>1.855</v>
+      </c>
+      <c r="Q769" s="3">
+        <v>44470</v>
+      </c>
+      <c r="R769">
+        <v>1.85</v>
+      </c>
+      <c r="S769" s="3">
+        <v>44470</v>
+      </c>
+      <c r="T769">
+        <v>1.8525</v>
+      </c>
+      <c r="U769" s="3">
+        <v>44470</v>
+      </c>
+      <c r="V769">
+        <v>1.87</v>
+      </c>
+      <c r="W769" s="3">
+        <v>44470</v>
+      </c>
+      <c r="X769">
+        <v>1.92</v>
+      </c>
+      <c r="Y769" s="3">
+        <v>44470</v>
+      </c>
+      <c r="Z769">
+        <v>1.97</v>
+      </c>
+      <c r="AA769" s="3">
+        <v>44470</v>
+      </c>
+      <c r="AB769">
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="AC769" s="3">
+        <v>44470</v>
+      </c>
+      <c r="AD769">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="770" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A770" s="3">
+        <v>44473</v>
+      </c>
+      <c r="B770">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="C770" s="3">
+        <v>44475</v>
+      </c>
+      <c r="D770">
+        <v>2.3149999999999999</v>
+      </c>
+      <c r="E770" s="3">
+        <v>44473</v>
+      </c>
+      <c r="F770">
+        <v>2.0575000000000001</v>
+      </c>
+      <c r="G770" s="3">
+        <v>44473</v>
+      </c>
+      <c r="H770">
+        <v>1.98</v>
+      </c>
+      <c r="I770" s="3">
+        <v>44473</v>
+      </c>
+      <c r="J770">
+        <v>1.9375</v>
+      </c>
+      <c r="K770" s="3">
+        <v>44473</v>
+      </c>
+      <c r="L770">
+        <v>1.9075</v>
+      </c>
+      <c r="M770" s="3">
+        <v>44473</v>
+      </c>
+      <c r="N770">
+        <v>1.885</v>
+      </c>
+      <c r="O770" s="3">
+        <v>44473</v>
+      </c>
+      <c r="P770">
+        <v>1.8774999999999999</v>
+      </c>
+      <c r="Q770" s="3">
+        <v>44473</v>
+      </c>
+      <c r="R770">
+        <v>1.87</v>
+      </c>
+      <c r="S770" s="3">
+        <v>44473</v>
+      </c>
+      <c r="T770">
+        <v>1.865</v>
+      </c>
+      <c r="U770" s="3">
+        <v>44473</v>
+      </c>
+      <c r="V770">
+        <v>1.88</v>
+      </c>
+      <c r="W770" s="3">
+        <v>44473</v>
+      </c>
+      <c r="X770">
+        <v>1.925</v>
+      </c>
+      <c r="Y770" s="3">
+        <v>44473</v>
+      </c>
+      <c r="Z770">
+        <v>1.9675</v>
+      </c>
+      <c r="AA770" s="3">
+        <v>44473</v>
+      </c>
+      <c r="AB770">
+        <v>2.0024999999999999</v>
+      </c>
+      <c r="AC770" s="3">
+        <v>44473</v>
+      </c>
+      <c r="AD770">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="771" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A771" s="3">
+        <v>44474</v>
+      </c>
+      <c r="B771">
+        <v>2.7475000000000001</v>
+      </c>
+      <c r="C771" s="3">
+        <v>44476</v>
+      </c>
+      <c r="D771">
+        <v>2.2949999999999999</v>
+      </c>
+      <c r="E771" s="3">
+        <v>44474</v>
+      </c>
+      <c r="F771">
+        <v>2.1875</v>
+      </c>
+      <c r="G771" s="3">
+        <v>44474</v>
+      </c>
+      <c r="H771">
+        <v>2.09</v>
+      </c>
+      <c r="I771" s="3">
+        <v>44474</v>
+      </c>
+      <c r="J771">
+        <v>2.0375000000000001</v>
+      </c>
+      <c r="K771" s="3">
+        <v>44474</v>
+      </c>
+      <c r="L771">
+        <v>2</v>
+      </c>
+      <c r="M771" s="3">
+        <v>44474</v>
+      </c>
+      <c r="N771">
+        <v>1.9675</v>
+      </c>
+      <c r="O771" s="3">
+        <v>44474</v>
+      </c>
+      <c r="P771">
+        <v>1.9550000000000001</v>
+      </c>
+      <c r="Q771" s="3">
+        <v>44474</v>
+      </c>
+      <c r="R771">
+        <v>1.9424999999999999</v>
+      </c>
+      <c r="S771" s="3">
+        <v>44474</v>
+      </c>
+      <c r="T771">
+        <v>1.9325000000000001</v>
+      </c>
+      <c r="U771" s="3">
+        <v>44474</v>
+      </c>
+      <c r="V771">
+        <v>1.9375</v>
+      </c>
+      <c r="W771" s="3">
+        <v>44474</v>
+      </c>
+      <c r="X771">
+        <v>1.9750000000000001</v>
+      </c>
+      <c r="Y771" s="3">
+        <v>44474</v>
+      </c>
+      <c r="Z771">
+        <v>2.0150000000000001</v>
+      </c>
+      <c r="AA771" s="3">
+        <v>44474</v>
+      </c>
+      <c r="AB771">
+        <v>2.0449999999999999</v>
+      </c>
+      <c r="AC771" s="3">
+        <v>44474</v>
+      </c>
+      <c r="AD771">
+        <v>2.0674999999999999</v>
+      </c>
+    </row>
+    <row r="772" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A772" s="3">
+        <v>44475</v>
+      </c>
+      <c r="B772">
+        <v>2.6949999999999998</v>
+      </c>
+      <c r="C772" s="3">
+        <v>44477</v>
+      </c>
+      <c r="D772">
+        <v>2.3250000000000002</v>
+      </c>
+      <c r="E772" s="3">
+        <v>44475</v>
+      </c>
+      <c r="F772">
+        <v>2.1324999999999998</v>
+      </c>
+      <c r="G772" s="3">
+        <v>44475</v>
+      </c>
+      <c r="H772">
+        <v>2.0375000000000001</v>
+      </c>
+      <c r="I772" s="3">
+        <v>44475</v>
+      </c>
+      <c r="J772">
+        <v>1.9849999999999999</v>
+      </c>
+      <c r="K772" s="3">
+        <v>44475</v>
+      </c>
+      <c r="L772">
+        <v>1.95</v>
+      </c>
+      <c r="M772" s="3">
+        <v>44475</v>
+      </c>
+      <c r="N772">
+        <v>1.925</v>
+      </c>
+      <c r="O772" s="3">
+        <v>44475</v>
+      </c>
+      <c r="P772">
+        <v>1.915</v>
+      </c>
+      <c r="Q772" s="3">
+        <v>44475</v>
+      </c>
+      <c r="R772">
+        <v>1.905</v>
+      </c>
+      <c r="S772" s="3">
+        <v>44475</v>
+      </c>
+      <c r="T772">
+        <v>1.9</v>
+      </c>
+      <c r="U772" s="3">
+        <v>44475</v>
+      </c>
+      <c r="V772">
+        <v>1.9075</v>
+      </c>
+      <c r="W772" s="3">
+        <v>44475</v>
+      </c>
+      <c r="X772">
+        <v>1.95</v>
+      </c>
+      <c r="Y772" s="3">
+        <v>44475</v>
+      </c>
+      <c r="Z772">
+        <v>1.9975000000000001</v>
+      </c>
+      <c r="AA772" s="3">
+        <v>44475</v>
+      </c>
+      <c r="AB772">
+        <v>2.0274999999999999</v>
+      </c>
+      <c r="AC772" s="3">
+        <v>44475</v>
+      </c>
+      <c r="AD772">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="773" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A773" s="3">
+        <v>44476</v>
+      </c>
+      <c r="B773">
+        <v>2.71</v>
+      </c>
+      <c r="C773" s="3">
+        <v>44480</v>
+      </c>
+      <c r="D773">
+        <v>2.3174999999999999</v>
+      </c>
+      <c r="E773" s="3">
+        <v>44476</v>
+      </c>
+      <c r="F773">
+        <v>2.1</v>
+      </c>
+      <c r="G773" s="3">
+        <v>44476</v>
+      </c>
+      <c r="H773">
+        <v>1.9975000000000001</v>
+      </c>
+      <c r="I773" s="3">
+        <v>44476</v>
+      </c>
+      <c r="J773">
+        <v>1.94</v>
+      </c>
+      <c r="K773" s="3">
+        <v>44476</v>
+      </c>
+      <c r="L773">
+        <v>1.9075</v>
+      </c>
+      <c r="M773" s="3">
+        <v>44476</v>
+      </c>
+      <c r="N773">
+        <v>1.885</v>
+      </c>
+      <c r="O773" s="3">
+        <v>44476</v>
+      </c>
+      <c r="P773">
+        <v>1.875</v>
+      </c>
+      <c r="Q773" s="3">
+        <v>44476</v>
+      </c>
+      <c r="R773">
+        <v>1.8675000000000002</v>
+      </c>
+      <c r="S773" s="3">
+        <v>44476</v>
+      </c>
+      <c r="T773">
+        <v>1.8675000000000002</v>
+      </c>
+      <c r="U773" s="3">
+        <v>44476</v>
+      </c>
+      <c r="V773">
+        <v>1.88</v>
+      </c>
+      <c r="W773" s="3">
+        <v>44476</v>
+      </c>
+      <c r="X773">
+        <v>1.9275</v>
+      </c>
+      <c r="Y773" s="3">
+        <v>44476</v>
+      </c>
+      <c r="Z773">
+        <v>1.9775</v>
+      </c>
+      <c r="AA773" s="3">
+        <v>44476</v>
+      </c>
+      <c r="AB773">
+        <v>2.0125000000000002</v>
+      </c>
+      <c r="AC773" s="3">
+        <v>44476</v>
+      </c>
+      <c r="AD773">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="774" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A774" s="3">
+        <v>44477</v>
+      </c>
+      <c r="B774">
+        <v>2.7549999999999999</v>
+      </c>
+      <c r="C774" s="3">
+        <v>44481</v>
+      </c>
+      <c r="D774">
+        <v>2.3275000000000001</v>
+      </c>
+      <c r="E774" s="3">
+        <v>44477</v>
+      </c>
+      <c r="F774">
+        <v>2.125</v>
+      </c>
+      <c r="G774" s="3">
+        <v>44477</v>
+      </c>
+      <c r="H774">
+        <v>2.02</v>
+      </c>
+      <c r="I774" s="3">
+        <v>44477</v>
+      </c>
+      <c r="J774">
+        <v>1.96</v>
+      </c>
+      <c r="K774" s="3">
+        <v>44477</v>
+      </c>
+      <c r="L774">
+        <v>1.925</v>
+      </c>
+      <c r="M774" s="3">
+        <v>44477</v>
+      </c>
+      <c r="N774">
+        <v>1.9024999999999999</v>
+      </c>
+      <c r="O774" s="3">
+        <v>44477</v>
+      </c>
+      <c r="P774">
+        <v>1.8925000000000001</v>
+      </c>
+      <c r="Q774" s="3">
+        <v>44477</v>
+      </c>
+      <c r="R774">
+        <v>1.8824999999999998</v>
+      </c>
+      <c r="S774" s="3">
+        <v>44477</v>
+      </c>
+      <c r="T774">
+        <v>1.8824999999999998</v>
+      </c>
+      <c r="U774" s="3">
+        <v>44477</v>
+      </c>
+      <c r="V774">
+        <v>1.895</v>
+      </c>
+      <c r="W774" s="3">
+        <v>44477</v>
+      </c>
+      <c r="X774">
+        <v>1.9424999999999999</v>
+      </c>
+      <c r="Y774" s="3">
+        <v>44477</v>
+      </c>
+      <c r="Z774">
+        <v>1.9925000000000002</v>
+      </c>
+      <c r="AA774" s="3">
+        <v>44477</v>
+      </c>
+      <c r="AB774">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="AC774" s="3">
+        <v>44477</v>
+      </c>
+      <c r="AD774">
+        <v>2.0575000000000001</v>
+      </c>
+    </row>
+    <row r="775" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A775" s="3">
+        <v>44480</v>
+      </c>
+      <c r="B775">
+        <v>2.79</v>
+      </c>
+      <c r="C775" s="3">
+        <v>44482</v>
+      </c>
+      <c r="D775">
+        <v>2.33</v>
+      </c>
+      <c r="E775" s="3">
+        <v>44480</v>
+      </c>
+      <c r="F775">
+        <v>2.1274999999999999</v>
+      </c>
+      <c r="G775" s="3">
+        <v>44480</v>
+      </c>
+      <c r="H775">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="I775" s="3">
+        <v>44480</v>
+      </c>
+      <c r="J775">
+        <v>1.97</v>
+      </c>
+      <c r="K775" s="3">
+        <v>44480</v>
+      </c>
+      <c r="L775">
+        <v>1.9350000000000001</v>
+      </c>
+      <c r="M775" s="3">
+        <v>44480</v>
+      </c>
+      <c r="N775">
+        <v>1.9125000000000001</v>
+      </c>
+      <c r="O775" s="3">
+        <v>44480</v>
+      </c>
+      <c r="P775">
+        <v>1.9024999999999999</v>
+      </c>
+      <c r="Q775" s="3">
+        <v>44480</v>
+      </c>
+      <c r="R775">
+        <v>1.895</v>
+      </c>
+      <c r="S775" s="3">
+        <v>44480</v>
+      </c>
+      <c r="T775">
+        <v>1.8925000000000001</v>
+      </c>
+      <c r="U775" s="3">
+        <v>44480</v>
+      </c>
+      <c r="V775">
+        <v>1.905</v>
+      </c>
+      <c r="W775" s="3">
+        <v>44480</v>
+      </c>
+      <c r="X775">
+        <v>1.9475</v>
+      </c>
+      <c r="Y775" s="3">
+        <v>44480</v>
+      </c>
+      <c r="Z775">
+        <v>1.9975000000000001</v>
+      </c>
+      <c r="AA775" s="3">
+        <v>44480</v>
+      </c>
+      <c r="AB775">
+        <v>2.0325000000000002</v>
+      </c>
+      <c r="AC775" s="3">
+        <v>44480</v>
+      </c>
+      <c r="AD775">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="776" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A776" s="3">
+        <v>44481</v>
+      </c>
+      <c r="B776">
+        <v>2.8075000000000001</v>
+      </c>
+      <c r="C776" s="3">
+        <v>44483</v>
+      </c>
+      <c r="D776">
+        <v>2.3224999999999998</v>
+      </c>
+      <c r="E776" s="3">
+        <v>44481</v>
+      </c>
+      <c r="F776">
+        <v>2.1425000000000001</v>
+      </c>
+      <c r="G776" s="3">
+        <v>44481</v>
+      </c>
+      <c r="H776">
+        <v>2.0474999999999999</v>
+      </c>
+      <c r="I776" s="3">
+        <v>44481</v>
+      </c>
+      <c r="J776">
+        <v>1.99</v>
+      </c>
+      <c r="K776" s="3">
+        <v>44481</v>
+      </c>
+      <c r="L776">
+        <v>1.9550000000000001</v>
+      </c>
+      <c r="M776" s="3">
+        <v>44481</v>
+      </c>
+      <c r="N776">
+        <v>1.9325000000000001</v>
+      </c>
+      <c r="O776" s="3">
+        <v>44481</v>
+      </c>
+      <c r="P776">
+        <v>1.9224999999999999</v>
+      </c>
+      <c r="Q776" s="3">
+        <v>44481</v>
+      </c>
+      <c r="R776">
+        <v>1.9125000000000001</v>
+      </c>
+      <c r="S776" s="3">
+        <v>44481</v>
+      </c>
+      <c r="T776">
+        <v>1.9125000000000001</v>
+      </c>
+      <c r="U776" s="3">
+        <v>44481</v>
+      </c>
+      <c r="V776">
+        <v>1.9275</v>
+      </c>
+      <c r="W776" s="3">
+        <v>44481</v>
+      </c>
+      <c r="X776">
+        <v>1.9775</v>
+      </c>
+      <c r="Y776" s="3">
+        <v>44481</v>
+      </c>
+      <c r="Z776">
+        <v>2.0325000000000002</v>
+      </c>
+      <c r="AA776" s="3">
+        <v>44481</v>
+      </c>
+      <c r="AB776">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="AC776" s="3">
+        <v>44481</v>
+      </c>
+      <c r="AD776">
+        <v>2.0975000000000001</v>
+      </c>
+    </row>
+    <row r="777" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A777" s="3">
+        <v>44482</v>
+      </c>
+      <c r="B777">
+        <v>2.8250000000000002</v>
+      </c>
+      <c r="C777" s="3">
+        <v>44484</v>
+      </c>
+      <c r="D777">
+        <v>2.3650000000000002</v>
+      </c>
+      <c r="E777" s="3">
+        <v>44482</v>
+      </c>
+      <c r="F777">
+        <v>2.1375000000000002</v>
+      </c>
+      <c r="G777" s="3">
+        <v>44482</v>
+      </c>
+      <c r="H777">
+        <v>2.04</v>
+      </c>
+      <c r="I777" s="3">
+        <v>44482</v>
+      </c>
+      <c r="J777">
+        <v>1.98</v>
+      </c>
+      <c r="K777" s="3">
+        <v>44482</v>
+      </c>
+      <c r="L777">
+        <v>1.9449999999999998</v>
+      </c>
+      <c r="M777" s="3">
+        <v>44482</v>
+      </c>
+      <c r="N777">
+        <v>1.92</v>
+      </c>
+      <c r="O777" s="3">
+        <v>44482</v>
+      </c>
+      <c r="P777">
+        <v>1.9100000000000001</v>
+      </c>
+      <c r="Q777" s="3">
+        <v>44482</v>
+      </c>
+      <c r="R777">
+        <v>1.9</v>
+      </c>
+      <c r="S777" s="3">
+        <v>44482</v>
+      </c>
+      <c r="T777">
+        <v>1.9</v>
+      </c>
+      <c r="U777" s="3">
+        <v>44482</v>
+      </c>
+      <c r="V777">
+        <v>1.9175</v>
+      </c>
+      <c r="W777" s="3">
+        <v>44482</v>
+      </c>
+      <c r="X777">
+        <v>1.9675</v>
+      </c>
+      <c r="Y777" s="3">
+        <v>44482</v>
+      </c>
+      <c r="Z777">
+        <v>2.0225</v>
+      </c>
+      <c r="AA777" s="3">
+        <v>44482</v>
+      </c>
+      <c r="AB777">
+        <v>2.0625</v>
+      </c>
+      <c r="AC777" s="3">
+        <v>44482</v>
+      </c>
+      <c r="AD777">
+        <v>2.0924999999999998</v>
+      </c>
+    </row>
+    <row r="778" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A778" s="3">
+        <v>44483</v>
+      </c>
+      <c r="B778">
+        <v>2.84</v>
+      </c>
+      <c r="C778" s="3">
+        <v>44487</v>
+      </c>
+      <c r="D778">
+        <v>2.41</v>
+      </c>
+      <c r="E778" s="3">
+        <v>44483</v>
+      </c>
+      <c r="F778">
+        <v>2.14</v>
+      </c>
+      <c r="G778" s="3">
+        <v>44483</v>
+      </c>
+      <c r="H778">
+        <v>2.0474999999999999</v>
+      </c>
+      <c r="I778" s="3">
+        <v>44483</v>
+      </c>
+      <c r="J778">
+        <v>1.9925000000000002</v>
+      </c>
+      <c r="K778" s="3">
+        <v>44483</v>
+      </c>
+      <c r="L778">
+        <v>1.9575</v>
+      </c>
+      <c r="M778" s="3">
+        <v>44483</v>
+      </c>
+      <c r="N778">
+        <v>1.9325000000000001</v>
+      </c>
+      <c r="O778" s="3">
+        <v>44483</v>
+      </c>
+      <c r="P778">
+        <v>1.92</v>
+      </c>
+      <c r="Q778" s="3">
+        <v>44483</v>
+      </c>
+      <c r="R778">
+        <v>1.9100000000000001</v>
+      </c>
+      <c r="S778" s="3">
+        <v>44483</v>
+      </c>
+      <c r="T778">
+        <v>1.9100000000000001</v>
+      </c>
+      <c r="U778" s="3">
+        <v>44483</v>
+      </c>
+      <c r="V778">
+        <v>1.9224999999999999</v>
+      </c>
+      <c r="W778" s="3">
+        <v>44483</v>
+      </c>
+      <c r="X778">
+        <v>1.97</v>
+      </c>
+      <c r="Y778" s="3">
+        <v>44483</v>
+      </c>
+      <c r="Z778">
+        <v>2.02</v>
+      </c>
+      <c r="AA778" s="3">
+        <v>44483</v>
+      </c>
+      <c r="AB778">
+        <v>2.0575000000000001</v>
+      </c>
+      <c r="AC778" s="3">
+        <v>44483</v>
+      </c>
+      <c r="AD778">
+        <v>2.085</v>
+      </c>
+    </row>
+    <row r="779" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A779" s="3">
+        <v>44484</v>
+      </c>
+      <c r="B779">
+        <v>2.8925000000000001</v>
+      </c>
+      <c r="C779" s="3">
+        <v>44488</v>
+      </c>
+      <c r="D779">
+        <v>2.415</v>
+      </c>
+      <c r="E779" s="3">
+        <v>44484</v>
+      </c>
+      <c r="F779">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="G779" s="3">
+        <v>44484</v>
+      </c>
+      <c r="H779">
+        <v>2.0874999999999999</v>
+      </c>
+      <c r="I779" s="3">
+        <v>44484</v>
+      </c>
+      <c r="J779">
+        <v>2.0325000000000002</v>
+      </c>
+      <c r="K779" s="3">
+        <v>44484</v>
+      </c>
+      <c r="L779">
+        <v>1.9975000000000001</v>
+      </c>
+      <c r="M779" s="3">
+        <v>44484</v>
+      </c>
+      <c r="N779">
+        <v>1.97</v>
+      </c>
+      <c r="O779" s="3">
+        <v>44484</v>
+      </c>
+      <c r="P779">
+        <v>1.96</v>
+      </c>
+      <c r="Q779" s="3">
+        <v>44484</v>
+      </c>
+      <c r="R779">
+        <v>1.9475</v>
+      </c>
+      <c r="S779" s="3">
+        <v>44484</v>
+      </c>
+      <c r="T779">
+        <v>1.9475</v>
+      </c>
+      <c r="U779" s="3">
+        <v>44484</v>
+      </c>
+      <c r="V779">
+        <v>1.96</v>
+      </c>
+      <c r="W779" s="3">
+        <v>44484</v>
+      </c>
+      <c r="X779">
+        <v>2.0024999999999999</v>
+      </c>
+      <c r="Y779" s="3">
+        <v>44484</v>
+      </c>
+      <c r="Z779">
+        <v>2.0550000000000002</v>
+      </c>
+      <c r="AA779" s="3">
+        <v>44484</v>
+      </c>
+      <c r="AB779">
+        <v>2.09</v>
+      </c>
+      <c r="AC779" s="3">
+        <v>44484</v>
+      </c>
+      <c r="AD779">
+        <v>2.1175000000000002</v>
+      </c>
+    </row>
+    <row r="780" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A780" s="3">
+        <v>44487</v>
+      </c>
+      <c r="B780">
+        <v>2.9550000000000001</v>
+      </c>
+      <c r="C780" s="3">
+        <v>44489</v>
+      </c>
+      <c r="D780">
+        <v>2.415</v>
+      </c>
+      <c r="E780" s="3">
+        <v>44487</v>
+      </c>
+      <c r="F780">
+        <v>2.2225000000000001</v>
+      </c>
+      <c r="G780" s="3">
+        <v>44487</v>
+      </c>
+      <c r="H780">
+        <v>2.1274999999999999</v>
+      </c>
+      <c r="I780" s="3">
+        <v>44487</v>
+      </c>
+      <c r="J780">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="K780" s="3">
+        <v>44487</v>
+      </c>
+      <c r="L780">
+        <v>2.0325000000000002</v>
+      </c>
+      <c r="M780" s="3">
+        <v>44487</v>
+      </c>
+      <c r="N780">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="O780" s="3">
+        <v>44487</v>
+      </c>
+      <c r="P780">
+        <v>1.9975000000000001</v>
+      </c>
+      <c r="Q780" s="3">
+        <v>44487</v>
+      </c>
+      <c r="R780">
+        <v>1.9849999999999999</v>
+      </c>
+      <c r="S780" s="3">
+        <v>44487</v>
+      </c>
+      <c r="T780">
+        <v>1.9849999999999999</v>
+      </c>
+      <c r="U780" s="3">
+        <v>44487</v>
+      </c>
+      <c r="V780">
+        <v>1.9975000000000001</v>
+      </c>
+      <c r="W780" s="3">
+        <v>44487</v>
+      </c>
+      <c r="X780">
+        <v>2.04</v>
+      </c>
+      <c r="Y780" s="3">
+        <v>44487</v>
+      </c>
+      <c r="Z780">
+        <v>2.0924999999999998</v>
+      </c>
+      <c r="AA780" s="3">
+        <v>44487</v>
+      </c>
+      <c r="AB780">
+        <v>2.125</v>
+      </c>
+      <c r="AC780" s="3">
+        <v>44487</v>
+      </c>
+      <c r="AD780">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="781" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A781" s="3">
+        <v>44488</v>
+      </c>
+      <c r="B781">
+        <v>2.98</v>
+      </c>
+      <c r="C781" s="3">
+        <v>44490</v>
+      </c>
+      <c r="D781">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="E781" s="3">
+        <v>44488</v>
+      </c>
+      <c r="F781">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="G781" s="3">
+        <v>44488</v>
+      </c>
+      <c r="H781">
+        <v>2.1225000000000001</v>
+      </c>
+      <c r="I781" s="3">
+        <v>44488</v>
+      </c>
+      <c r="J781">
+        <v>2.0625</v>
+      </c>
+      <c r="K781" s="3">
+        <v>44488</v>
+      </c>
+      <c r="L781">
+        <v>2.0274999999999999</v>
+      </c>
+      <c r="M781" s="3">
+        <v>44488</v>
+      </c>
+      <c r="N781">
+        <v>2.0074999999999998</v>
+      </c>
+      <c r="O781" s="3">
+        <v>44488</v>
+      </c>
+      <c r="P781">
+        <v>1.9950000000000001</v>
+      </c>
+      <c r="Q781" s="3">
+        <v>44488</v>
+      </c>
+      <c r="R781">
+        <v>1.9849999999999999</v>
+      </c>
+      <c r="S781" s="3">
+        <v>44488</v>
+      </c>
+      <c r="T781">
+        <v>1.9849999999999999</v>
+      </c>
+      <c r="U781" s="3">
+        <v>44488</v>
+      </c>
+      <c r="V781">
+        <v>2</v>
+      </c>
+      <c r="W781" s="3">
+        <v>44488</v>
+      </c>
+      <c r="X781">
+        <v>2.0449999999999999</v>
+      </c>
+      <c r="Y781" s="3">
+        <v>44488</v>
+      </c>
+      <c r="Z781">
+        <v>2.1</v>
+      </c>
+      <c r="AA781" s="3">
+        <v>44488</v>
+      </c>
+      <c r="AB781">
+        <v>2.1349999999999998</v>
+      </c>
+      <c r="AC781" s="3">
+        <v>44488</v>
+      </c>
+      <c r="AD781">
+        <v>2.1625000000000001</v>
+      </c>
+    </row>
+    <row r="782" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A782" s="3">
+        <v>44489</v>
+      </c>
+      <c r="B782">
+        <v>3.0074999999999998</v>
+      </c>
+      <c r="C782" s="3">
+        <v>44491</v>
+      </c>
+      <c r="D782">
+        <v>2.5</v>
+      </c>
+      <c r="E782" s="3">
+        <v>44489</v>
+      </c>
+      <c r="F782">
+        <v>2.2075</v>
+      </c>
+      <c r="G782" s="3">
+        <v>44489</v>
+      </c>
+      <c r="H782">
+        <v>2.1074999999999999</v>
+      </c>
+      <c r="I782" s="3">
+        <v>44489</v>
+      </c>
+      <c r="J782">
+        <v>2.0474999999999999</v>
+      </c>
+      <c r="K782" s="3">
+        <v>44489</v>
+      </c>
+      <c r="L782">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="M782" s="3">
+        <v>44489</v>
+      </c>
+      <c r="N782">
+        <v>1.9875</v>
+      </c>
+      <c r="O782" s="3">
+        <v>44489</v>
+      </c>
+      <c r="P782">
+        <v>1.9775</v>
+      </c>
+      <c r="Q782" s="3">
+        <v>44489</v>
+      </c>
+      <c r="R782">
+        <v>1.9675</v>
+      </c>
+      <c r="S782" s="3">
+        <v>44489</v>
+      </c>
+      <c r="T782">
+        <v>1.97</v>
+      </c>
+      <c r="U782" s="3">
+        <v>44489</v>
+      </c>
+      <c r="V782">
+        <v>1.9849999999999999</v>
+      </c>
+      <c r="W782" s="3">
+        <v>44489</v>
+      </c>
+      <c r="X782">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="Y782" s="3">
+        <v>44489</v>
+      </c>
+      <c r="Z782">
+        <v>2.0874999999999999</v>
+      </c>
+      <c r="AA782" s="3">
+        <v>44489</v>
+      </c>
+      <c r="AB782">
+        <v>2.12</v>
+      </c>
+      <c r="AC782" s="3">
+        <v>44489</v>
+      </c>
+      <c r="AD782">
+        <v>2.1425000000000001</v>
+      </c>
+    </row>
+    <row r="783" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A783" s="3">
+        <v>44490</v>
+      </c>
+      <c r="B783">
+        <v>3.0350000000000001</v>
+      </c>
+      <c r="C783" s="3">
+        <v>44494</v>
+      </c>
+      <c r="D783">
+        <v>2.5300000000000002</v>
+      </c>
+      <c r="E783" s="3">
+        <v>44490</v>
+      </c>
+      <c r="F783">
+        <v>2.25</v>
+      </c>
+      <c r="G783" s="3">
+        <v>44490</v>
+      </c>
+      <c r="H783">
+        <v>2.1549999999999998</v>
+      </c>
+      <c r="I783" s="3">
+        <v>44490</v>
+      </c>
+      <c r="J783">
+        <v>2.0975000000000001</v>
+      </c>
+      <c r="K783" s="3">
+        <v>44490</v>
+      </c>
+      <c r="L783">
+        <v>2.06</v>
+      </c>
+      <c r="M783" s="3">
+        <v>44490</v>
+      </c>
+      <c r="N783">
+        <v>2.0375000000000001</v>
+      </c>
+      <c r="O783" s="3">
+        <v>44490</v>
+      </c>
+      <c r="P783">
+        <v>2.0274999999999999</v>
+      </c>
+      <c r="Q783" s="3">
+        <v>44490</v>
+      </c>
+      <c r="R783">
+        <v>2.02</v>
+      </c>
+      <c r="S783" s="3">
+        <v>44490</v>
+      </c>
+      <c r="T783">
+        <v>2.0225</v>
+      </c>
+      <c r="U783" s="3">
+        <v>44490</v>
+      </c>
+      <c r="V783">
+        <v>2.04</v>
+      </c>
+      <c r="W783" s="3">
+        <v>44490</v>
+      </c>
+      <c r="X783">
+        <v>2.0874999999999999</v>
+      </c>
+      <c r="Y783" s="3">
+        <v>44490</v>
+      </c>
+      <c r="Z783">
+        <v>2.1475</v>
+      </c>
+      <c r="AA783" s="3">
+        <v>44490</v>
+      </c>
+      <c r="AB783">
+        <v>2.1825000000000001</v>
+      </c>
+      <c r="AC783" s="3">
+        <v>44490</v>
+      </c>
+      <c r="AD783">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="784" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A784" s="3">
+        <v>44491</v>
+      </c>
+      <c r="B784">
+        <v>3.0825</v>
+      </c>
+      <c r="E784" s="3">
+        <v>44491</v>
+      </c>
+      <c r="F784">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G784" s="3">
+        <v>44491</v>
+      </c>
+      <c r="H784">
+        <v>2.2050000000000001</v>
+      </c>
+      <c r="I784" s="3">
+        <v>44491</v>
+      </c>
+      <c r="J784">
+        <v>2.1475</v>
+      </c>
+      <c r="K784" s="3">
+        <v>44491</v>
+      </c>
+      <c r="L784">
+        <v>2.11</v>
+      </c>
+      <c r="M784" s="3">
+        <v>44491</v>
+      </c>
+      <c r="N784">
+        <v>2.0874999999999999</v>
+      </c>
+      <c r="O784" s="3">
+        <v>44491</v>
+      </c>
+      <c r="P784">
+        <v>2.0775000000000001</v>
+      </c>
+      <c r="Q784" s="3">
+        <v>44491</v>
+      </c>
+      <c r="R784">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="S784" s="3">
+        <v>44491</v>
+      </c>
+      <c r="T784">
+        <v>2.0724999999999998</v>
+      </c>
+      <c r="U784" s="3">
+        <v>44491</v>
+      </c>
+      <c r="V784">
+        <v>2.09</v>
+      </c>
+      <c r="W784" s="3">
+        <v>44491</v>
+      </c>
+      <c r="X784">
+        <v>2.1375000000000002</v>
+      </c>
+      <c r="Y784" s="3">
+        <v>44491</v>
+      </c>
+      <c r="Z784">
+        <v>2.1974999999999998</v>
+      </c>
+      <c r="AA784" s="3">
+        <v>44491</v>
+      </c>
+      <c r="AB784">
+        <v>2.2324999999999999</v>
+      </c>
+      <c r="AC784" s="3">
+        <v>44491</v>
+      </c>
+      <c r="AD784">
+        <v>2.2574999999999998</v>
+      </c>
+    </row>
+    <row r="785" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A785" s="3">
+        <v>44494</v>
+      </c>
+      <c r="B785">
+        <v>3.13</v>
+      </c>
+      <c r="E785" s="3">
+        <v>44494</v>
+      </c>
+      <c r="F785">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G785" s="3">
+        <v>44494</v>
+      </c>
+      <c r="H785">
+        <v>2.2225000000000001</v>
+      </c>
+      <c r="I785" s="3">
+        <v>44494</v>
+      </c>
+      <c r="J785">
+        <v>2.1625000000000001</v>
+      </c>
+      <c r="K785" s="3">
+        <v>44494</v>
+      </c>
+      <c r="L785">
+        <v>2.1274999999999999</v>
+      </c>
+      <c r="M785" s="3">
+        <v>44494</v>
+      </c>
+      <c r="N785">
+        <v>2.1074999999999999</v>
+      </c>
+      <c r="O785" s="3">
+        <v>44494</v>
+      </c>
+      <c r="P785">
+        <v>2.0975000000000001</v>
+      </c>
+      <c r="Q785" s="3">
+        <v>44494</v>
+      </c>
+      <c r="R785">
+        <v>2.0924999999999998</v>
+      </c>
+      <c r="S785" s="3">
+        <v>44494</v>
+      </c>
+      <c r="T785">
+        <v>2.0950000000000002</v>
+      </c>
+      <c r="U785" s="3">
+        <v>44494</v>
+      </c>
+      <c r="V785">
+        <v>2.1124999999999998</v>
+      </c>
+      <c r="W785" s="3">
+        <v>44494</v>
+      </c>
+      <c r="X785">
+        <v>2.1625000000000001</v>
+      </c>
+      <c r="Y785" s="3">
+        <v>44494</v>
+      </c>
+      <c r="Z785">
+        <v>2.2225000000000001</v>
+      </c>
+      <c r="AA785" s="3">
+        <v>44494</v>
+      </c>
+      <c r="AB785">
+        <v>2.2574999999999998</v>
+      </c>
+      <c r="AC785" s="3">
+        <v>44494</v>
+      </c>
+      <c r="AD785">
+        <v>2.2824999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>